<commit_message>
Corrected "Skip backwards through the album using swipe" Expected from "Tracks returned in random order" to the actual behaviour "Tracks returned in the reverse order they were played"
</commit_message>
<xml_diff>
--- a/Mobile/Manual/Unified Mobile Functional Test Template .xlsx
+++ b/Mobile/Manual/Unified Mobile Functional Test Template .xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="852">
   <si>
     <t>Test date:</t>
   </si>
@@ -5383,6 +5383,9 @@
     <t>[1] Play artist Radio_x000D_
 [2] (Android only) when moved to chugger, press back</t>
   </si>
+  <si>
+    <t>Tracks returned in the reverse order they were played</t>
+  </si>
 </sst>
 </file>
 
@@ -5681,7 +5684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -5836,9 +5839,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5954,6 +5954,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6397,35 +6403,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="12.75"/>
-    <row r="3" spans="1:19" s="65" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="97" t="s">
+    <row r="3" spans="1:19" s="64" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="65" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -6462,25 +6468,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="91" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="98" t="s">
+    <row r="4" spans="1:19" s="90" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="91" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="90" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -6510,20 +6516,20 @@
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="1:19" s="47" customFormat="1" ht="12.75">
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:19" s="47" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="95" t="s">
         <v>677</v>
       </c>
-      <c r="C8" s="94"/>
+      <c r="C8" s="95"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:19" s="47" customFormat="1" ht="51">
@@ -6539,7 +6545,7 @@
       <c r="E9" s="47" t="s">
         <v>680</v>
       </c>
-      <c r="I9" s="90"/>
+      <c r="I9" s="89"/>
     </row>
     <row r="10" spans="1:19" s="47" customFormat="1" ht="12.75">
       <c r="D10" s="8"/>
@@ -6554,24 +6560,24 @@
       <c r="D11" s="8" t="s">
         <v>682</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="63" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="54" customFormat="1" ht="12.75">
+    <row r="12" spans="1:19" s="53" customFormat="1" ht="12.75">
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:19" s="54" customFormat="1" ht="12.75">
-      <c r="B13" s="54" t="s">
+    <row r="13" spans="1:19" s="53" customFormat="1" ht="12.75">
+      <c r="B13" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="53" t="s">
         <v>705</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>706</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="53" t="s">
         <v>707</v>
       </c>
     </row>
@@ -6579,10 +6585,10 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:19" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="94"/>
+      <c r="C15" s="95"/>
     </row>
     <row r="16" spans="1:19" s="2" customFormat="1" ht="30">
       <c r="B16" s="2" t="s">
@@ -6663,7 +6669,7 @@
       <c r="D22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="88" t="s">
+      <c r="E22" s="87" t="s">
         <v>832</v>
       </c>
     </row>
@@ -6674,7 +6680,7 @@
       <c r="D23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="89" t="s">
+      <c r="E23" s="88" t="s">
         <v>832</v>
       </c>
     </row>
@@ -6906,10 +6912,10 @@
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="94"/>
+      <c r="C43" s="95"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -7105,21 +7111,21 @@
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
     </row>
-    <row r="56" spans="2:10" s="76" customFormat="1">
-      <c r="B56" s="76" t="s">
+    <row r="56" spans="2:10" s="75" customFormat="1">
+      <c r="B56" s="75" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>806</v>
       </c>
-      <c r="E56" s="77" t="s">
+      <c r="E56" s="76" t="s">
         <v>807</v>
       </c>
-      <c r="F56" s="77"/>
-      <c r="G56" s="77"/>
-      <c r="H56" s="77"/>
-      <c r="I56" s="77"/>
-      <c r="J56" s="77"/>
+      <c r="F56" s="76"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="76"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="76"/>
     </row>
     <row r="57" spans="2:10" s="2" customFormat="1" ht="30">
       <c r="B57" s="2" t="s">
@@ -7200,11 +7206,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="2:10" s="84" customFormat="1">
-      <c r="D64" s="53" t="s">
+    <row r="64" spans="2:10" s="83" customFormat="1">
+      <c r="D64" s="52" t="s">
         <v>819</v>
       </c>
-      <c r="E64" s="53" t="s">
+      <c r="E64" s="52" t="s">
         <v>820</v>
       </c>
     </row>
@@ -7216,7 +7222,7 @@
       <c r="C66" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D66" s="53" t="s">
+      <c r="D66" s="52" t="s">
         <v>687</v>
       </c>
       <c r="E66" s="10" t="s">
@@ -7262,11 +7268,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="84" customFormat="1">
-      <c r="D72" s="53" t="s">
+    <row r="72" spans="1:5" s="83" customFormat="1">
+      <c r="D72" s="52" t="s">
         <v>819</v>
       </c>
-      <c r="E72" s="53" t="s">
+      <c r="E72" s="52" t="s">
         <v>820</v>
       </c>
     </row>
@@ -7293,11 +7299,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="83" customFormat="1">
-      <c r="D76" s="53" t="s">
+    <row r="76" spans="1:5" s="82" customFormat="1">
+      <c r="D76" s="52" t="s">
         <v>819</v>
       </c>
-      <c r="E76" s="53" t="s">
+      <c r="E76" s="52" t="s">
         <v>820</v>
       </c>
     </row>
@@ -7306,9 +7312,9 @@
       <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A78" s="95"/>
-      <c r="B78" s="95"/>
-      <c r="C78" s="95"/>
+      <c r="A78" s="96"/>
+      <c r="B78" s="96"/>
+      <c r="C78" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -7359,35 +7365,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="12.75"/>
-    <row r="3" spans="1:19" s="65" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="97" t="s">
+    <row r="3" spans="1:19" s="64" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="65" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -7424,25 +7430,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="91" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="98" t="s">
+    <row r="4" spans="1:19" s="90" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="91" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="90" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -7472,17 +7478,17 @@
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="94"/>
+      <c r="C7" s="95"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
@@ -7500,10 +7506,10 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="94"/>
+      <c r="C9" s="95"/>
       <c r="D9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -7526,7 +7532,7 @@
       <c r="D11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="76" t="s">
+      <c r="E11" s="75" t="s">
         <v>805</v>
       </c>
     </row>
@@ -7562,7 +7568,7 @@
       <c r="D14" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="54" t="s">
         <v>708</v>
       </c>
     </row>
@@ -7573,7 +7579,7 @@
       <c r="D15" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="54" t="s">
         <v>710</v>
       </c>
     </row>
@@ -7584,7 +7590,7 @@
       <c r="D16" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="54" t="s">
         <v>709</v>
       </c>
     </row>
@@ -7598,7 +7604,7 @@
       <c r="D17" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="54" t="s">
         <v>711</v>
       </c>
     </row>
@@ -7664,7 +7670,7 @@
       <c r="C23" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="54" t="s">
         <v>712</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -7675,7 +7681,7 @@
       <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="55" t="s">
+      <c r="D24" s="54" t="s">
         <v>713</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -7686,7 +7692,7 @@
       <c r="B25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="54" t="s">
         <v>714</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -7697,7 +7703,7 @@
       <c r="B26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="55" t="s">
+      <c r="D26" s="54" t="s">
         <v>715</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -7708,7 +7714,7 @@
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="54" t="s">
         <v>716</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -7765,7 +7771,7 @@
       <c r="D32" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="54" t="s">
         <v>717</v>
       </c>
       <c r="I32" s="10"/>
@@ -7935,10 +7941,10 @@
       <c r="J48" s="10"/>
     </row>
     <row r="49" spans="2:18" s="2" customFormat="1" ht="93" customHeight="1">
-      <c r="B49" s="94" t="s">
+      <c r="B49" s="95" t="s">
         <v>718</v>
       </c>
-      <c r="C49" s="94"/>
+      <c r="C49" s="95"/>
       <c r="D49" s="2" t="s">
         <v>174</v>
       </c>
@@ -7960,7 +7966,7 @@
       <c r="R49" s="10"/>
     </row>
     <row r="50" spans="2:18" s="2" customFormat="1">
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="54" t="s">
         <v>26</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -8074,10 +8080,10 @@
       <c r="R55" s="10"/>
     </row>
     <row r="56" spans="2:18" s="2" customFormat="1">
-      <c r="B56" s="94" t="s">
+      <c r="B56" s="95" t="s">
         <v>184</v>
       </c>
-      <c r="C56" s="94"/>
+      <c r="C56" s="95"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
@@ -8092,8 +8098,8 @@
       <c r="Q56" s="10"/>
       <c r="R56" s="10"/>
     </row>
-    <row r="57" spans="2:18" s="76" customFormat="1" ht="135" customHeight="1">
-      <c r="B57" s="76" t="s">
+    <row r="57" spans="2:18" s="75" customFormat="1" ht="135" customHeight="1">
+      <c r="B57" s="75" t="s">
         <v>26</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -8105,22 +8111,22 @@
       <c r="E57" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F57" s="77"/>
-      <c r="G57" s="77"/>
-      <c r="H57" s="77"/>
-      <c r="I57" s="77"/>
-      <c r="J57" s="77"/>
-      <c r="K57" s="77"/>
-      <c r="L57" s="77"/>
-      <c r="M57" s="77"/>
-      <c r="N57" s="77"/>
-      <c r="O57" s="77"/>
-      <c r="P57" s="77"/>
-      <c r="Q57" s="77"/>
-      <c r="R57" s="77"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="76"/>
+      <c r="M57" s="76"/>
+      <c r="N57" s="76"/>
+      <c r="O57" s="76"/>
+      <c r="P57" s="76"/>
+      <c r="Q57" s="76"/>
+      <c r="R57" s="76"/>
     </row>
     <row r="58" spans="2:18" s="2" customFormat="1">
-      <c r="B58" s="76"/>
+      <c r="B58" s="75"/>
       <c r="D58" s="2" t="s">
         <v>187</v>
       </c>
@@ -8290,7 +8296,7 @@
       <c r="C69" s="7" t="s">
         <v>808</v>
       </c>
-      <c r="D69" s="76" t="s">
+      <c r="D69" s="75" t="s">
         <v>809</v>
       </c>
       <c r="E69" s="17" t="s">
@@ -8360,9 +8366,9 @@
       <c r="R72" s="1"/>
     </row>
     <row r="73" spans="1:18" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A73" s="95"/>
-      <c r="B73" s="95"/>
-      <c r="C73" s="95"/>
+      <c r="A73" s="96"/>
+      <c r="B73" s="96"/>
+      <c r="C73" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -8413,35 +8419,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="12.75"/>
-    <row r="3" spans="1:19" s="65" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="97" t="s">
+    <row r="3" spans="1:19" s="64" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="65" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -8478,25 +8484,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="91" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="99" t="s">
+    <row r="4" spans="1:19" s="90" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="91" t="s">
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="90" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -8526,21 +8532,21 @@
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="8" spans="1:19" s="2" customFormat="1">
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="C9" s="94"/>
+      <c r="C9" s="95"/>
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" ht="33" customHeight="1">
       <c r="B10" s="2" t="s">
@@ -8660,24 +8666,24 @@
         <v>720</v>
       </c>
     </row>
-    <row r="21" spans="2:10" s="74" customFormat="1">
+    <row r="21" spans="2:10" s="73" customFormat="1">
       <c r="E21" s="17"/>
     </row>
-    <row r="22" spans="2:10" s="74" customFormat="1" ht="25.5">
-      <c r="B22" s="74" t="s">
+    <row r="22" spans="2:10" s="73" customFormat="1" ht="25.5">
+      <c r="B22" s="73" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>785</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="73" t="s">
         <v>786</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="2:10" s="74" customFormat="1">
+    <row r="23" spans="2:10" s="73" customFormat="1">
       <c r="E23" s="17"/>
     </row>
     <row r="24" spans="2:10" s="2" customFormat="1" ht="25.5">
@@ -8698,28 +8704,28 @@
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="2:10" s="2" customFormat="1">
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="95" t="s">
         <v>227</v>
       </c>
-      <c r="C26" s="94"/>
+      <c r="C26" s="95"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="2:10" s="76" customFormat="1" ht="63.75">
-      <c r="B27" s="76" t="s">
+    <row r="27" spans="2:10" s="75" customFormat="1" ht="63.75">
+      <c r="B27" s="75" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="54" t="s">
         <v>721</v>
       </c>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
     </row>
     <row r="28" spans="2:10" s="2" customFormat="1" ht="60">
       <c r="D28" s="2" t="s">
@@ -8915,7 +8921,7 @@
       <c r="C45" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="D45" s="55" t="s">
+      <c r="D45" s="54" t="s">
         <v>724</v>
       </c>
       <c r="E45" s="17" t="s">
@@ -8935,7 +8941,7 @@
     <row r="46" spans="2:18" s="2" customFormat="1">
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
-      <c r="K46" s="56"/>
+      <c r="K46" s="55"/>
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
@@ -9150,7 +9156,7 @@
       <c r="C59" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="D59" s="55" t="s">
+      <c r="D59" s="54" t="s">
         <v>725</v>
       </c>
       <c r="E59" s="17" t="s">
@@ -9181,14 +9187,14 @@
       <c r="R60" s="1"/>
     </row>
     <row r="61" spans="2:18" s="2" customFormat="1" ht="89.25">
-      <c r="B61" s="94" t="s">
+      <c r="B61" s="95" t="s">
         <v>263</v>
       </c>
-      <c r="C61" s="94"/>
+      <c r="C61" s="95"/>
       <c r="D61" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="55" t="s">
+      <c r="E61" s="54" t="s">
         <v>726</v>
       </c>
       <c r="F61" s="10"/>
@@ -9209,7 +9215,7 @@
       <c r="D62" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E62" s="55" t="s">
+      <c r="E62" s="54" t="s">
         <v>727</v>
       </c>
       <c r="F62" s="10"/>
@@ -9425,10 +9431,10 @@
       <c r="R72" s="1"/>
     </row>
     <row r="73" spans="2:18" s="2" customFormat="1" ht="51" customHeight="1">
-      <c r="B73" s="94" t="s">
+      <c r="B73" s="95" t="s">
         <v>279</v>
       </c>
-      <c r="C73" s="94"/>
+      <c r="C73" s="95"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
@@ -9453,7 +9459,7 @@
       <c r="D74" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E74" s="92" t="s">
+      <c r="E74" s="91" t="s">
         <v>842</v>
       </c>
     </row>
@@ -9461,7 +9467,7 @@
       <c r="D75" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E75" s="92" t="s">
+      <c r="E75" s="91" t="s">
         <v>842</v>
       </c>
     </row>
@@ -9469,7 +9475,7 @@
       <c r="D76" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E76" s="55" t="s">
+      <c r="E76" s="54" t="s">
         <v>231</v>
       </c>
     </row>
@@ -9483,7 +9489,7 @@
       <c r="D78" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E78" s="92" t="s">
+      <c r="E78" s="91" t="s">
         <v>842</v>
       </c>
     </row>
@@ -9497,7 +9503,7 @@
       <c r="D79" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="E79" s="92" t="s">
+      <c r="E79" s="91" t="s">
         <v>843</v>
       </c>
     </row>
@@ -9515,10 +9521,10 @@
       <c r="R80" s="1"/>
     </row>
     <row r="81" spans="1:18" ht="41.25" customHeight="1">
-      <c r="B81" s="94" t="s">
+      <c r="B81" s="95" t="s">
         <v>288</v>
       </c>
-      <c r="C81" s="94"/>
+      <c r="C81" s="95"/>
     </row>
     <row r="82" spans="1:18" s="8" customFormat="1" ht="25.5">
       <c r="B82" s="8" t="s">
@@ -9545,9 +9551,9 @@
       <c r="R82" s="1"/>
     </row>
     <row r="84" spans="1:18" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A84" s="95"/>
-      <c r="B84" s="95"/>
-      <c r="C84" s="95"/>
+      <c r="A84" s="96"/>
+      <c r="B84" s="96"/>
+      <c r="C84" s="96"/>
       <c r="I84" s="23"/>
       <c r="J84" s="23"/>
       <c r="K84" s="23"/>
@@ -9609,35 +9615,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="12.75"/>
-    <row r="3" spans="1:19" s="65" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="97" t="s">
+    <row r="3" spans="1:19" s="64" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="65" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -9674,25 +9680,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="91" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="98" t="s">
+    <row r="4" spans="1:19" s="90" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="91" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="90" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -9721,59 +9727,59 @@
       <c r="R4" s="4"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="96" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" ht="12.75"/>
-    <row r="8" spans="1:19" s="66" customFormat="1" ht="12.75">
-      <c r="B8" s="94" t="s">
+    <row r="8" spans="1:19" s="65" customFormat="1" ht="12.75">
+      <c r="B8" s="95" t="s">
         <v>765</v>
       </c>
-      <c r="C8" s="94"/>
-    </row>
-    <row r="9" spans="1:19" s="66" customFormat="1" ht="12.75">
-      <c r="B9" s="66" t="s">
+      <c r="C8" s="95"/>
+    </row>
+    <row r="9" spans="1:19" s="65" customFormat="1" ht="12.75">
+      <c r="B9" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="65" t="s">
         <v>759</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="65" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="66" customFormat="1" ht="25.5">
-      <c r="B10" s="66" t="s">
+    <row r="10" spans="1:19" s="65" customFormat="1" ht="25.5">
+      <c r="B10" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="66" t="s">
+      <c r="C10" s="66"/>
+      <c r="D10" s="65" t="s">
         <v>761</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="65" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="66" customFormat="1" ht="25.5">
-      <c r="B11" s="66" t="s">
+    <row r="11" spans="1:19" s="65" customFormat="1" ht="25.5">
+      <c r="B11" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="65" t="s">
         <v>763</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="65" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="66" customFormat="1" ht="12.75"/>
+    <row r="12" spans="1:19" s="65" customFormat="1" ht="12.75"/>
     <row r="13" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="95" t="s">
         <v>766</v>
       </c>
-      <c r="C13" s="94"/>
+      <c r="C13" s="95"/>
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1">
       <c r="B14" s="2" t="s">
@@ -9876,10 +9882,10 @@
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="95" t="s">
         <v>767</v>
       </c>
-      <c r="C24" s="94"/>
+      <c r="C24" s="95"/>
       <c r="D24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -9920,7 +9926,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="2:10" s="2" customFormat="1">
-      <c r="B28" s="75"/>
+      <c r="B28" s="74"/>
       <c r="D28" s="2" t="s">
         <v>311</v>
       </c>
@@ -9992,10 +9998,10 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B33" s="94" t="s">
+      <c r="B33" s="95" t="s">
         <v>768</v>
       </c>
-      <c r="C33" s="94"/>
+      <c r="C33" s="95"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
@@ -10118,10 +10124,10 @@
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="95" t="s">
         <v>769</v>
       </c>
-      <c r="C43" s="94"/>
+      <c r="C43" s="95"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
@@ -10252,10 +10258,10 @@
       <c r="R52" s="10"/>
     </row>
     <row r="53" spans="2:18" s="2" customFormat="1" ht="34.5" customHeight="1">
-      <c r="B53" s="94" t="s">
+      <c r="B53" s="95" t="s">
         <v>770</v>
       </c>
-      <c r="C53" s="94"/>
+      <c r="C53" s="95"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
@@ -10292,7 +10298,7 @@
       <c r="C55" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="D55" s="76" t="s">
+      <c r="D55" s="75" t="s">
         <v>813</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -10460,10 +10466,10 @@
       <c r="R62" s="1"/>
     </row>
     <row r="63" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B63" s="94" t="s">
+      <c r="B63" s="95" t="s">
         <v>771</v>
       </c>
-      <c r="C63" s="94"/>
+      <c r="C63" s="95"/>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
@@ -10587,10 +10593,10 @@
       <c r="R68" s="1"/>
     </row>
     <row r="69" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B69" s="94" t="s">
+      <c r="B69" s="95" t="s">
         <v>772</v>
       </c>
-      <c r="C69" s="94"/>
+      <c r="C69" s="95"/>
       <c r="E69" s="1"/>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
@@ -10630,7 +10636,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="2:18" s="66" customFormat="1" ht="12.75">
+    <row r="71" spans="2:18" s="65" customFormat="1" ht="12.75">
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
@@ -10645,11 +10651,11 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="2:18" s="66" customFormat="1" ht="12.75">
-      <c r="B72" s="94" t="s">
+    <row r="72" spans="2:18" s="65" customFormat="1" ht="12.75">
+      <c r="B72" s="95" t="s">
         <v>773</v>
       </c>
-      <c r="C72" s="94"/>
+      <c r="C72" s="95"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
       <c r="I72" s="1"/>
@@ -10663,17 +10669,17 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="2:18" s="66" customFormat="1" ht="12.75">
-      <c r="B73" s="66" t="s">
+    <row r="73" spans="2:18" s="65" customFormat="1" ht="12.75">
+      <c r="B73" s="65" t="s">
         <v>42</v>
       </c>
       <c r="C73" s="24" t="s">
         <v>774</v>
       </c>
-      <c r="D73" s="73" t="s">
+      <c r="D73" s="72" t="s">
         <v>775</v>
       </c>
-      <c r="E73" s="68" t="s">
+      <c r="E73" s="67" t="s">
         <v>776</v>
       </c>
       <c r="I73" s="1"/>
@@ -10687,10 +10693,10 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="2:18" s="66" customFormat="1" ht="12.75">
+    <row r="74" spans="2:18" s="65" customFormat="1" ht="12.75">
       <c r="C74" s="8"/>
-      <c r="D74" s="69"/>
-      <c r="E74" s="70" t="s">
+      <c r="D74" s="68"/>
+      <c r="E74" s="69" t="s">
         <v>777</v>
       </c>
       <c r="I74" s="1"/>
@@ -10704,10 +10710,10 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="2:18" s="66" customFormat="1" ht="12.75">
+    <row r="75" spans="2:18" s="65" customFormat="1" ht="12.75">
       <c r="C75" s="8"/>
-      <c r="D75" s="69"/>
-      <c r="E75" s="70" t="s">
+      <c r="D75" s="68"/>
+      <c r="E75" s="69" t="s">
         <v>790</v>
       </c>
       <c r="I75" s="1"/>
@@ -10721,12 +10727,12 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="2:18" s="66" customFormat="1" ht="12.75">
+    <row r="76" spans="2:18" s="65" customFormat="1" ht="12.75">
       <c r="C76" s="8"/>
-      <c r="D76" s="73" t="s">
+      <c r="D76" s="72" t="s">
         <v>778</v>
       </c>
-      <c r="E76" s="68" t="s">
+      <c r="E76" s="67" t="s">
         <v>776</v>
       </c>
       <c r="I76" s="1"/>
@@ -10740,10 +10746,10 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="2:18" s="66" customFormat="1" ht="12.75">
+    <row r="77" spans="2:18" s="65" customFormat="1" ht="12.75">
       <c r="C77" s="8"/>
-      <c r="D77" s="71"/>
-      <c r="E77" s="72" t="s">
+      <c r="D77" s="70"/>
+      <c r="E77" s="71" t="s">
         <v>777</v>
       </c>
       <c r="I77" s="1"/>
@@ -10757,7 +10763,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="2:18" s="66" customFormat="1" ht="12.75">
+    <row r="78" spans="2:18" s="65" customFormat="1" ht="12.75">
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
@@ -10772,7 +10778,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="2:18" s="66" customFormat="1" ht="12.75">
+    <row r="79" spans="2:18" s="65" customFormat="1" ht="12.75">
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
@@ -10787,7 +10793,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="2:18" s="66" customFormat="1" ht="12.75">
+    <row r="80" spans="2:18" s="65" customFormat="1" ht="12.75">
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
@@ -10818,9 +10824,9 @@
       <c r="R81" s="1"/>
     </row>
     <row r="82" spans="1:18" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A82" s="95"/>
-      <c r="B82" s="95"/>
-      <c r="C82" s="95"/>
+      <c r="A82" s="96"/>
+      <c r="B82" s="96"/>
+      <c r="C82" s="96"/>
       <c r="I82" s="23"/>
       <c r="J82" s="23"/>
       <c r="K82" s="23"/>
@@ -10887,35 +10893,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="12.75"/>
-    <row r="3" spans="1:19" s="65" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="97" t="s">
+    <row r="3" spans="1:19" s="64" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="65" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -10953,11 +10959,11 @@
       </c>
     </row>
     <row r="4" spans="1:19" s="5" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -11000,18 +11006,18 @@
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="96" t="s">
         <v>346</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="8" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="103" t="s">
         <v>347</v>
       </c>
-      <c r="C8" s="102"/>
+      <c r="C8" s="103"/>
       <c r="E8" s="1"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -11166,10 +11172,10 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="2:10" s="2" customFormat="1" ht="32.25" customHeight="1">
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="103" t="s">
         <v>366</v>
       </c>
-      <c r="C22" s="102"/>
+      <c r="C22" s="103"/>
       <c r="E22" s="18"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -11382,7 +11388,7 @@
       <c r="J39" s="10"/>
     </row>
     <row r="40" spans="2:10" s="2" customFormat="1">
-      <c r="D40" s="57" t="s">
+      <c r="D40" s="56" t="s">
         <v>735</v>
       </c>
       <c r="E40" s="17" t="s">
@@ -11409,7 +11415,7 @@
       <c r="C42" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="D42" s="57" t="s">
+      <c r="D42" s="56" t="s">
         <v>391</v>
       </c>
       <c r="E42" s="17" t="s">
@@ -11422,7 +11428,7 @@
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="2:10" s="2" customFormat="1">
-      <c r="D43" s="57" t="s">
+      <c r="D43" s="56" t="s">
         <v>393</v>
       </c>
       <c r="E43" s="17" t="s">
@@ -11434,18 +11440,18 @@
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="2:10" s="57" customFormat="1" ht="25.5">
-      <c r="D44" s="57" t="s">
+    <row r="44" spans="2:10" s="56" customFormat="1" ht="25.5">
+      <c r="D44" s="56" t="s">
         <v>737</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>736</v>
       </c>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
     </row>
     <row r="45" spans="2:10" s="2" customFormat="1">
       <c r="E45" s="17"/>
@@ -11537,10 +11543,10 @@
       <c r="J51" s="10"/>
     </row>
     <row r="52" spans="2:18" s="2" customFormat="1" ht="19.5" customHeight="1">
-      <c r="B52" s="102" t="s">
+      <c r="B52" s="103" t="s">
         <v>401</v>
       </c>
-      <c r="C52" s="102"/>
+      <c r="C52" s="103"/>
       <c r="E52" s="8"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
@@ -11773,7 +11779,7 @@
       <c r="R63" s="10"/>
     </row>
     <row r="64" spans="2:18" s="2" customFormat="1">
-      <c r="D64" s="75" t="s">
+      <c r="D64" s="74" t="s">
         <v>791</v>
       </c>
       <c r="E64" s="17" t="s">
@@ -11794,7 +11800,7 @@
       <c r="R64" s="10"/>
     </row>
     <row r="65" spans="2:18" s="2" customFormat="1" ht="25.5">
-      <c r="D65" s="75" t="s">
+      <c r="D65" s="74" t="s">
         <v>792</v>
       </c>
       <c r="E65" s="8" t="s">
@@ -11983,10 +11989,10 @@
       <c r="R74" s="1"/>
     </row>
     <row r="75" spans="2:18" s="2" customFormat="1" ht="19.5" customHeight="1">
-      <c r="B75" s="102" t="s">
+      <c r="B75" s="103" t="s">
         <v>413</v>
       </c>
-      <c r="C75" s="102"/>
+      <c r="C75" s="103"/>
       <c r="E75" s="17"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
@@ -12068,7 +12074,7 @@
       <c r="C79" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="D79" s="57" t="s">
+      <c r="D79" s="56" t="s">
         <v>742</v>
       </c>
       <c r="E79" s="15" t="s">
@@ -12417,7 +12423,7 @@
       <c r="R97" s="1"/>
     </row>
     <row r="98" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="D98" s="57" t="s">
+      <c r="D98" s="56" t="s">
         <v>735</v>
       </c>
       <c r="E98" s="17" t="s">
@@ -12558,10 +12564,10 @@
       <c r="R105" s="1"/>
     </row>
     <row r="106" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B106" s="102" t="s">
+      <c r="B106" s="103" t="s">
         <v>428</v>
       </c>
-      <c r="C106" s="102"/>
+      <c r="C106" s="103"/>
       <c r="D106" s="8"/>
       <c r="E106" s="8"/>
       <c r="I106" s="1"/>
@@ -12887,10 +12893,10 @@
       <c r="R121" s="1"/>
     </row>
     <row r="122" spans="2:18" s="2" customFormat="1" ht="32.25" customHeight="1">
-      <c r="B122" s="102" t="s">
+      <c r="B122" s="103" t="s">
         <v>455</v>
       </c>
-      <c r="C122" s="102"/>
+      <c r="C122" s="103"/>
       <c r="E122" s="18"/>
       <c r="F122" s="10"/>
       <c r="G122" s="10"/>
@@ -12930,7 +12936,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="2:18" s="92" customFormat="1">
+    <row r="124" spans="2:18" s="91" customFormat="1">
       <c r="C124" s="17"/>
       <c r="D124" s="17"/>
       <c r="E124" s="46"/>
@@ -12945,8 +12951,8 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="2:18" s="92" customFormat="1" ht="30">
-      <c r="B125" s="92" t="s">
+    <row r="125" spans="2:18" s="91" customFormat="1" ht="30">
+      <c r="B125" s="91" t="s">
         <v>42</v>
       </c>
       <c r="C125" s="7" t="s">
@@ -13320,10 +13326,10 @@
       <c r="R142" s="1"/>
     </row>
     <row r="143" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B143" s="102" t="s">
+      <c r="B143" s="103" t="s">
         <v>462</v>
       </c>
-      <c r="C143" s="102"/>
+      <c r="C143" s="103"/>
       <c r="D143" s="8"/>
       <c r="E143" s="8"/>
       <c r="I143" s="1"/>
@@ -13648,7 +13654,7 @@
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="2:18" s="92" customFormat="1" ht="12.75">
+    <row r="159" spans="2:18" s="91" customFormat="1" ht="12.75">
       <c r="C159" s="7"/>
       <c r="D159" s="8"/>
       <c r="E159" s="8"/>
@@ -13664,10 +13670,10 @@
       <c r="R159" s="1"/>
     </row>
     <row r="160" spans="2:18" s="2" customFormat="1" ht="32.25" customHeight="1">
-      <c r="B160" s="102" t="s">
+      <c r="B160" s="103" t="s">
         <v>831</v>
       </c>
-      <c r="C160" s="102"/>
+      <c r="C160" s="103"/>
       <c r="E160" s="18"/>
       <c r="F160" s="10"/>
       <c r="G160" s="10"/>
@@ -13879,9 +13885,9 @@
       <c r="R170" s="1"/>
     </row>
     <row r="171" spans="1:18" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A171" s="95"/>
-      <c r="B171" s="95"/>
-      <c r="C171" s="95"/>
+      <c r="A171" s="96"/>
+      <c r="B171" s="96"/>
+      <c r="C171" s="96"/>
       <c r="I171" s="23"/>
       <c r="J171" s="23"/>
       <c r="K171" s="23"/>
@@ -13946,35 +13952,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="12.75"/>
-    <row r="3" spans="1:19" s="65" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="97" t="s">
+    <row r="3" spans="1:19" s="64" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="65" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -14011,25 +14017,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="91" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="98" t="s">
+    <row r="4" spans="1:19" s="90" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="91" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="90" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -14059,18 +14065,18 @@
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="96" t="s">
         <v>467</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="8" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="105" t="s">
         <v>468</v>
       </c>
-      <c r="C8" s="104"/>
+      <c r="C8" s="105"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -14299,11 +14305,11 @@
       <c r="R26" s="2"/>
     </row>
     <row r="27" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="105" t="s">
         <v>496</v>
       </c>
-      <c r="C27" s="104"/>
-      <c r="D27" s="58"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="57"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -14707,7 +14713,7 @@
       <c r="B54" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D54" s="87" t="s">
+      <c r="D54" s="86" t="s">
         <v>794</v>
       </c>
       <c r="E54" s="8" t="s">
@@ -14729,16 +14735,16 @@
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="E55" s="9"/>
-      <c r="I55" s="86"/>
-      <c r="J55" s="86"/>
-      <c r="K55" s="86"/>
-      <c r="L55" s="86"/>
-      <c r="M55" s="86"/>
-      <c r="N55" s="86"/>
-      <c r="O55" s="86"/>
-      <c r="P55" s="86"/>
-      <c r="Q55" s="86"/>
-      <c r="R55" s="86"/>
+      <c r="I55" s="85"/>
+      <c r="J55" s="85"/>
+      <c r="K55" s="85"/>
+      <c r="L55" s="85"/>
+      <c r="M55" s="85"/>
+      <c r="N55" s="85"/>
+      <c r="O55" s="85"/>
+      <c r="P55" s="85"/>
+      <c r="Q55" s="85"/>
+      <c r="R55" s="85"/>
       <c r="S55"/>
       <c r="T55"/>
       <c r="U55"/>
@@ -15749,10 +15755,10 @@
     </row>
     <row r="56" spans="1:1025" ht="15" customHeight="1">
       <c r="A56"/>
-      <c r="B56" s="102" t="s">
+      <c r="B56" s="103" t="s">
         <v>522</v>
       </c>
-      <c r="C56" s="102"/>
+      <c r="C56" s="103"/>
       <c r="D56" s="9"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
@@ -34199,10 +34205,10 @@
     </row>
     <row r="74" spans="1:1025" ht="15" customHeight="1">
       <c r="A74"/>
-      <c r="B74" s="102" t="s">
+      <c r="B74" s="103" t="s">
         <v>531</v>
       </c>
-      <c r="C74" s="102"/>
+      <c r="C74" s="103"/>
       <c r="S74"/>
       <c r="T74"/>
       <c r="U74"/>
@@ -49479,10 +49485,10 @@
     </row>
     <row r="89" spans="1:1025" ht="37.5" customHeight="1">
       <c r="A89"/>
-      <c r="B89" s="103" t="s">
+      <c r="B89" s="104" t="s">
         <v>543</v>
       </c>
-      <c r="C89" s="103"/>
+      <c r="C89" s="104"/>
       <c r="S89"/>
       <c r="T89"/>
       <c r="U89"/>
@@ -65923,10 +65929,10 @@
     </row>
     <row r="105" spans="1:1025" ht="28.5" customHeight="1">
       <c r="A105"/>
-      <c r="B105" s="103" t="s">
+      <c r="B105" s="104" t="s">
         <v>546</v>
       </c>
-      <c r="C105" s="103"/>
+      <c r="C105" s="104"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
       <c r="F105"/>
@@ -81257,11 +81263,11 @@
       <c r="AMK119"/>
     </row>
     <row r="120" spans="1:1025" s="2" customFormat="1" ht="29.25" customHeight="1">
-      <c r="B120" s="102" t="s">
+      <c r="B120" s="103" t="s">
         <v>547</v>
       </c>
-      <c r="C120" s="102"/>
-      <c r="D120" s="57"/>
+      <c r="C120" s="103"/>
+      <c r="D120" s="56"/>
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
@@ -81280,7 +81286,7 @@
       <c r="C121" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="D121" s="59" t="s">
+      <c r="D121" s="58" t="s">
         <v>746</v>
       </c>
       <c r="E121" s="8" t="s">
@@ -81301,7 +81307,7 @@
       <c r="B122" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D122" s="59" t="s">
+      <c r="D122" s="58" t="s">
         <v>747</v>
       </c>
       <c r="E122" s="8" t="s">
@@ -81322,7 +81328,7 @@
       <c r="B123" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D123" s="57" t="s">
+      <c r="D123" s="56" t="s">
         <v>552</v>
       </c>
       <c r="E123" s="2" t="s">
@@ -81364,7 +81370,7 @@
       <c r="B125" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D125" s="57" t="s">
+      <c r="D125" s="56" t="s">
         <v>556</v>
       </c>
       <c r="E125" s="8" t="s">
@@ -81385,7 +81391,7 @@
       <c r="B126" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D126" s="57" t="s">
+      <c r="D126" s="56" t="s">
         <v>558</v>
       </c>
       <c r="E126" s="8" t="s">
@@ -81406,7 +81412,7 @@
       <c r="B127" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D127" s="57" t="s">
+      <c r="D127" s="56" t="s">
         <v>686</v>
       </c>
       <c r="E127" s="2" t="s">
@@ -81636,7 +81642,7 @@
       <c r="C138" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="D138" s="57" t="s">
+      <c r="D138" s="56" t="s">
         <v>576</v>
       </c>
       <c r="E138" s="1" t="s">
@@ -81667,9 +81673,9 @@
       <c r="R139" s="1"/>
     </row>
     <row r="140" spans="1:18" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A140" s="95"/>
-      <c r="B140" s="95"/>
-      <c r="C140" s="95"/>
+      <c r="A140" s="96"/>
+      <c r="B140" s="96"/>
+      <c r="C140" s="96"/>
       <c r="I140" s="23"/>
       <c r="J140" s="23"/>
       <c r="K140" s="23"/>
@@ -81761,8 +81767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98:E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -81787,35 +81793,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="12.75"/>
-    <row r="3" spans="1:19" s="65" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="97" t="s">
+    <row r="3" spans="1:19" s="64" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="65" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="64" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -81852,25 +81858,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="91" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="98" t="s">
+    <row r="4" spans="1:19" s="90" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="91" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="90" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -81900,13 +81906,13 @@
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="12.75"/>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="96" t="s">
         <v>748</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
     </row>
     <row r="7" spans="1:19" s="2" customFormat="1" ht="12.75">
       <c r="A7" s="51"/>
@@ -81917,10 +81923,10 @@
     </row>
     <row r="8" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="51"/>
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="105" t="s">
         <v>468</v>
       </c>
-      <c r="C8" s="104"/>
+      <c r="C8" s="105"/>
       <c r="D8" s="51"/>
       <c r="E8" s="51"/>
       <c r="F8" s="10"/>
@@ -81929,7 +81935,7 @@
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="51"/>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -81941,20 +81947,20 @@
       <c r="E9" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
+      <c r="B10" s="93"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="51"/>
-      <c r="B11" s="51"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="7" t="s">
         <v>471</v>
       </c>
@@ -81967,7 +81973,7 @@
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" ht="25.5">
       <c r="A12" s="51"/>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -81982,14 +81988,14 @@
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" ht="12.75">
       <c r="A13" s="51"/>
-      <c r="B13" s="51"/>
+      <c r="B13" s="93"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" ht="25.5">
       <c r="A14" s="51"/>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -82004,7 +82010,7 @@
     </row>
     <row r="15" spans="1:19" s="2" customFormat="1" ht="33.75" customHeight="1">
       <c r="A15" s="51"/>
-      <c r="B15" s="51"/>
+      <c r="B15" s="93"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8" t="s">
         <v>480</v>
@@ -82015,7 +82021,7 @@
     </row>
     <row r="16" spans="1:19" s="2" customFormat="1" ht="12.75">
       <c r="A16" s="51"/>
-      <c r="B16" s="51"/>
+      <c r="B16" s="93"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8" t="s">
         <v>481</v>
@@ -82026,7 +82032,7 @@
     </row>
     <row r="17" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A17" s="51"/>
-      <c r="B17" s="51"/>
+      <c r="B17" s="93"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8" t="s">
         <v>483</v>
@@ -82037,14 +82043,14 @@
     </row>
     <row r="18" spans="1:18" s="2" customFormat="1" ht="12.75">
       <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" ht="25.5">
       <c r="A19" s="51"/>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -82059,7 +82065,7 @@
     </row>
     <row r="20" spans="1:18" s="2" customFormat="1" ht="12.75">
       <c r="A20" s="51"/>
-      <c r="B20" s="51"/>
+      <c r="B20" s="93"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
         <v>488</v>
@@ -82181,19 +82187,19 @@
     </row>
     <row r="27" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="51"/>
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="105" t="s">
         <v>496</v>
       </c>
-      <c r="C27" s="104"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="51"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="93"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A28" s="51"/>
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -82210,7 +82216,7 @@
     </row>
     <row r="29" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A29" s="51"/>
-      <c r="B29" s="51"/>
+      <c r="B29" s="93"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -82219,7 +82225,7 @@
     </row>
     <row r="30" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="51"/>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -82236,7 +82242,7 @@
     </row>
     <row r="31" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A31" s="51"/>
-      <c r="B31" s="51"/>
+      <c r="B31" s="93"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
         <v>499</v>
@@ -82249,8 +82255,8 @@
     </row>
     <row r="32" spans="1:18" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A32" s="51"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
+      <c r="B32" s="93"/>
+      <c r="C32" s="93"/>
       <c r="D32" s="8" t="s">
         <v>500</v>
       </c>
@@ -82262,7 +82268,7 @@
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A33" s="51"/>
-      <c r="B33" s="51"/>
+      <c r="B33" s="93"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="17"/>
@@ -82271,7 +82277,7 @@
     </row>
     <row r="34" spans="1:18" s="2" customFormat="1" ht="25.5">
       <c r="A34" s="51"/>
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -82288,14 +82294,14 @@
     </row>
     <row r="35" spans="1:18" s="2" customFormat="1" ht="12.75">
       <c r="A35" s="51"/>
-      <c r="B35" s="51"/>
+      <c r="B35" s="93"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:18" s="2" customFormat="1" ht="25.5">
       <c r="A36" s="51"/>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -82312,7 +82318,7 @@
     </row>
     <row r="37" spans="1:18" s="2" customFormat="1" ht="33.75" customHeight="1">
       <c r="A37" s="51"/>
-      <c r="B37" s="51"/>
+      <c r="B37" s="93"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8" t="s">
         <v>480</v>
@@ -82325,7 +82331,7 @@
     </row>
     <row r="38" spans="1:18" s="2" customFormat="1">
       <c r="A38" s="51"/>
-      <c r="B38" s="51"/>
+      <c r="B38" s="93"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8" t="s">
         <v>481</v>
@@ -82338,7 +82344,7 @@
     </row>
     <row r="39" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A39" s="51"/>
-      <c r="B39" s="51"/>
+      <c r="B39" s="93"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -82347,7 +82353,7 @@
     </row>
     <row r="40" spans="1:18" s="2" customFormat="1" ht="33.75" customHeight="1">
       <c r="A40" s="51"/>
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="7" t="s">
@@ -82364,8 +82370,8 @@
     </row>
     <row r="41" spans="1:18" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A41" s="51"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="51"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
       <c r="D41" s="1" t="s">
         <v>505</v>
       </c>
@@ -82377,8 +82383,8 @@
     </row>
     <row r="42" spans="1:18" s="2" customFormat="1">
       <c r="A42" s="51"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="93"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="I42" s="10"/>
@@ -82386,7 +82392,7 @@
     </row>
     <row r="43" spans="1:18" s="2" customFormat="1" ht="25.5">
       <c r="A43" s="51"/>
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -82403,7 +82409,7 @@
     </row>
     <row r="44" spans="1:18" s="2" customFormat="1" ht="19.5" customHeight="1">
       <c r="A44" s="51"/>
-      <c r="B44" s="51"/>
+      <c r="B44" s="93"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8" t="s">
         <v>488</v>
@@ -82618,7 +82624,7 @@
       <c r="R53" s="10"/>
     </row>
     <row r="54" spans="2:18" ht="25.5">
-      <c r="D54" s="87" t="s">
+      <c r="D54" s="86" t="s">
         <v>850</v>
       </c>
       <c r="E54" s="8" t="s">
@@ -82652,10 +82658,10 @@
       <c r="R55" s="10"/>
     </row>
     <row r="56" spans="2:18" ht="15" customHeight="1">
-      <c r="B56" s="104" t="s">
+      <c r="B56" s="105" t="s">
         <v>522</v>
       </c>
-      <c r="C56" s="104"/>
+      <c r="C56" s="105"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
       <c r="K56" s="10"/>
@@ -82722,7 +82728,7 @@
         <v>691</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>524</v>
+        <v>851</v>
       </c>
       <c r="I59" s="10"/>
       <c r="J59" s="10"/>
@@ -82766,7 +82772,7 @@
         <v>693</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>524</v>
+        <v>851</v>
       </c>
       <c r="I61" s="10"/>
       <c r="J61" s="10"/>
@@ -82884,7 +82890,7 @@
         <v>698</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>524</v>
+        <v>851</v>
       </c>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
@@ -82918,7 +82924,7 @@
         <v>525</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>524</v>
+        <v>851</v>
       </c>
     </row>
     <row r="70" spans="2:18">
@@ -82930,13 +82936,15 @@
         <v>526</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="71" spans="2:18">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
-      <c r="E71" s="9"/>
+      <c r="E71" s="9" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="72" spans="2:18">
       <c r="B72" s="8" t="s">
@@ -82958,10 +82966,10 @@
       <c r="E73" s="9"/>
     </row>
     <row r="74" spans="2:18" ht="15" customHeight="1">
-      <c r="B74" s="104" t="s">
+      <c r="B74" s="105" t="s">
         <v>531</v>
       </c>
-      <c r="C74" s="104"/>
+      <c r="C74" s="105"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
     </row>
@@ -83117,10 +83125,10 @@
       </c>
     </row>
     <row r="89" spans="2:18" ht="37.5" customHeight="1">
-      <c r="B89" s="105" t="s">
+      <c r="B89" s="106" t="s">
         <v>694</v>
       </c>
-      <c r="C89" s="105"/>
+      <c r="C89" s="106"/>
     </row>
     <row r="90" spans="2:18">
       <c r="B90" s="8" t="s">
@@ -83157,7 +83165,7 @@
         <v>691</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>524</v>
+        <v>851</v>
       </c>
     </row>
     <row r="93" spans="2:18">
@@ -83191,7 +83199,7 @@
         <v>693</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>524</v>
+        <v>851</v>
       </c>
     </row>
     <row r="95" spans="2:18">
@@ -83257,7 +83265,7 @@
         <v>698</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>524</v>
+        <v>851</v>
       </c>
     </row>
     <row r="101" spans="2:5">
@@ -83281,7 +83289,7 @@
         <v>699</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>524</v>
+        <v>851</v>
       </c>
     </row>
     <row r="103" spans="2:5">
@@ -83299,13 +83307,15 @@
     <row r="104" spans="2:5">
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
-      <c r="E104" s="9"/>
+      <c r="E104" s="9" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="105" spans="2:5" ht="28.5" customHeight="1">
-      <c r="B105" s="105" t="s">
+      <c r="B105" s="106" t="s">
         <v>695</v>
       </c>
-      <c r="C105" s="105"/>
+      <c r="C105" s="106"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
     </row>
@@ -83458,10 +83468,12 @@
       </c>
     </row>
     <row r="120" spans="2:18" s="2" customFormat="1" ht="29.25" customHeight="1">
-      <c r="B120" s="104" t="s">
+      <c r="B120" s="105" t="s">
         <v>547</v>
       </c>
-      <c r="C120" s="104"/>
+      <c r="C120" s="105"/>
+      <c r="D120" s="93"/>
+      <c r="E120" s="93"/>
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
@@ -83474,13 +83486,13 @@
       <c r="R120" s="1"/>
     </row>
     <row r="121" spans="2:18" s="2" customFormat="1" ht="30">
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="93" t="s">
         <v>26</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D121" s="93" t="s">
         <v>549</v>
       </c>
       <c r="E121" s="8" t="s">
@@ -83871,9 +83883,9 @@
       <c r="C140" s="9"/>
     </row>
     <row r="141" spans="1:18" s="6" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A141" s="95"/>
-      <c r="B141" s="95"/>
-      <c r="C141" s="95"/>
+      <c r="A141" s="96"/>
+      <c r="B141" s="96"/>
+      <c r="C141" s="96"/>
       <c r="I141" s="23"/>
       <c r="J141" s="23"/>
       <c r="K141" s="23"/>
@@ -83937,15 +83949,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106"/>
+      <c r="B1" s="107"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="107" t="s">
         <v>578</v>
       </c>
-      <c r="E1" s="106"/>
+      <c r="E1" s="107"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -83970,11 +83982,11 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
       <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
@@ -84024,25 +84036,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="91" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="98" t="s">
+    <row r="4" spans="1:19" s="90" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="91" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="90" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -84083,11 +84095,11 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:19" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="108" t="s">
         <v>579</v>
       </c>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="108"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -84112,10 +84124,10 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="104" t="s">
         <v>580</v>
       </c>
-      <c r="C8" s="103"/>
+      <c r="C8" s="104"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -84134,10 +84146,10 @@
       <c r="C9" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="61" t="s">
         <v>751</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="61" t="s">
         <v>752</v>
       </c>
       <c r="I9" s="2"/>
@@ -84189,23 +84201,23 @@
       <c r="R11" s="2"/>
       <c r="S11" s="9"/>
     </row>
-    <row r="12" spans="1:19" s="86" customFormat="1">
+    <row r="12" spans="1:19" s="85" customFormat="1">
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="85"/>
-      <c r="K12" s="85"/>
-      <c r="L12" s="85"/>
-      <c r="M12" s="85"/>
-      <c r="N12" s="85"/>
-      <c r="O12" s="85"/>
-      <c r="P12" s="85"/>
-      <c r="Q12" s="85"/>
-      <c r="R12" s="85"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="84"/>
+      <c r="L12" s="84"/>
+      <c r="M12" s="84"/>
+      <c r="N12" s="84"/>
+      <c r="O12" s="84"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="84"/>
+      <c r="R12" s="84"/>
       <c r="S12" s="9"/>
     </row>
-    <row r="13" spans="1:19" s="86" customFormat="1">
-      <c r="B13" s="86" t="s">
+    <row r="13" spans="1:19" s="85" customFormat="1">
+      <c r="B13" s="85" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="30" t="s">
@@ -84217,35 +84229,35 @@
       <c r="E13" s="44" t="s">
         <v>830</v>
       </c>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="85"/>
-      <c r="M13" s="85"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85"/>
-      <c r="R13" s="85"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="84"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="84"/>
+      <c r="N13" s="84"/>
+      <c r="O13" s="84"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="84"/>
+      <c r="R13" s="84"/>
       <c r="S13" s="9"/>
     </row>
-    <row r="14" spans="1:19" s="86" customFormat="1">
+    <row r="14" spans="1:19" s="85" customFormat="1">
       <c r="D14" s="44" t="s">
         <v>824</v>
       </c>
       <c r="E14" s="44" t="s">
         <v>825</v>
       </c>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="L14" s="85"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="84"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="84"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="84"/>
+      <c r="P14" s="84"/>
+      <c r="Q14" s="84"/>
+      <c r="R14" s="84"/>
       <c r="S14" s="9"/>
     </row>
     <row r="15" spans="1:19" s="10" customFormat="1">
@@ -84261,10 +84273,10 @@
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="104" t="s">
         <v>585</v>
       </c>
-      <c r="C16" s="103"/>
+      <c r="C16" s="104"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -84286,7 +84298,7 @@
       <c r="D17" s="10" t="s">
         <v>587</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="62" t="s">
         <v>755</v>
       </c>
       <c r="I17" s="2"/>
@@ -84307,7 +84319,7 @@
       <c r="D18" s="10" t="s">
         <v>589</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="62" t="s">
         <v>756</v>
       </c>
       <c r="I18" s="2"/>
@@ -84427,7 +84439,7 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="2:18" s="10" customFormat="1">
-      <c r="B24" s="93" t="s">
+      <c r="B24" s="92" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="10" t="s">
@@ -84447,23 +84459,23 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="2:18" s="93" customFormat="1">
-      <c r="I25" s="92"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="92"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
-      <c r="O25" s="92"/>
-      <c r="P25" s="92"/>
-      <c r="Q25" s="92"/>
-      <c r="R25" s="92"/>
+    <row r="25" spans="2:18" s="92" customFormat="1">
+      <c r="I25" s="91"/>
+      <c r="J25" s="91"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="91"/>
+      <c r="O25" s="91"/>
+      <c r="P25" s="91"/>
+      <c r="Q25" s="91"/>
+      <c r="R25" s="91"/>
     </row>
     <row r="26" spans="2:18" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="B26" s="103" t="s">
+      <c r="B26" s="104" t="s">
         <v>599</v>
       </c>
-      <c r="C26" s="103"/>
+      <c r="C26" s="104"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -85080,16 +85092,16 @@
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
-      <c r="I57" s="82"/>
-      <c r="J57" s="82"/>
-      <c r="K57" s="81"/>
-      <c r="L57" s="81"/>
-      <c r="M57" s="81"/>
-      <c r="N57" s="81"/>
-      <c r="O57" s="81"/>
-      <c r="P57" s="81"/>
-      <c r="Q57" s="81"/>
-      <c r="R57" s="81"/>
+      <c r="I57" s="81"/>
+      <c r="J57" s="81"/>
+      <c r="K57" s="80"/>
+      <c r="L57" s="80"/>
+      <c r="M57" s="80"/>
+      <c r="N57" s="80"/>
+      <c r="O57" s="80"/>
+      <c r="P57" s="80"/>
+      <c r="Q57" s="80"/>
+      <c r="R57" s="80"/>
     </row>
     <row r="58" spans="2:18">
       <c r="B58" s="9" t="s">
@@ -85148,16 +85160,16 @@
       <c r="E60" s="9" t="s">
         <v>754</v>
       </c>
-      <c r="I60" s="62"/>
-      <c r="J60" s="62"/>
-      <c r="K60" s="61"/>
-      <c r="L60" s="61"/>
-      <c r="M60" s="61"/>
-      <c r="N60" s="61"/>
-      <c r="O60" s="61"/>
-      <c r="P60" s="61"/>
-      <c r="Q60" s="61"/>
-      <c r="R60" s="61"/>
+      <c r="I60" s="61"/>
+      <c r="J60" s="61"/>
+      <c r="K60" s="60"/>
+      <c r="L60" s="60"/>
+      <c r="M60" s="60"/>
+      <c r="N60" s="60"/>
+      <c r="O60" s="60"/>
+      <c r="P60" s="60"/>
+      <c r="Q60" s="60"/>
+      <c r="R60" s="60"/>
     </row>
     <row r="61" spans="2:18">
       <c r="B61" s="9"/>
@@ -85274,10 +85286,10 @@
       <c r="R66" s="2"/>
     </row>
     <row r="67" spans="2:18" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="B67" s="103" t="s">
+      <c r="B67" s="104" t="s">
         <v>639</v>
       </c>
-      <c r="C67" s="103"/>
+      <c r="C67" s="104"/>
       <c r="D67" s="9"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
@@ -85386,10 +85398,10 @@
     </row>
     <row r="76" spans="2:18" s="32" customFormat="1"/>
     <row r="77" spans="2:18" s="32" customFormat="1">
-      <c r="B77" s="108" t="s">
+      <c r="B77" s="109" t="s">
         <v>779</v>
       </c>
-      <c r="C77" s="103"/>
+      <c r="C77" s="104"/>
       <c r="D77" s="22"/>
       <c r="E77" s="22"/>
     </row>
@@ -85429,10 +85441,10 @@
       <c r="R79" s="10"/>
     </row>
     <row r="80" spans="2:18" ht="15" customHeight="1">
-      <c r="B80" s="108" t="s">
+      <c r="B80" s="109" t="s">
         <v>780</v>
       </c>
-      <c r="C80" s="103"/>
+      <c r="C80" s="104"/>
       <c r="D80" s="10"/>
       <c r="E80" s="10"/>
       <c r="I80" s="10"/>
@@ -85631,10 +85643,10 @@
       </c>
     </row>
     <row r="97" spans="2:5" ht="15" customHeight="1">
-      <c r="B97" s="103" t="s">
+      <c r="B97" s="104" t="s">
         <v>729</v>
       </c>
-      <c r="C97" s="103"/>
+      <c r="C97" s="104"/>
     </row>
     <row r="98" spans="2:5" ht="45">
       <c r="B98" s="22" t="s">
@@ -85662,202 +85674,202 @@
       <c r="D100" s="9"/>
     </row>
     <row r="101" spans="2:5">
-      <c r="B101" s="108" t="s">
+      <c r="B101" s="109" t="s">
         <v>781</v>
       </c>
-      <c r="C101" s="103"/>
+      <c r="C101" s="104"/>
       <c r="D101" s="9"/>
     </row>
     <row r="102" spans="2:5" ht="45">
-      <c r="B102" s="60" t="s">
+      <c r="B102" s="59" t="s">
         <v>26</v>
       </c>
       <c r="D102" s="44" t="s">
         <v>738</v>
       </c>
-      <c r="E102" s="60" t="s">
+      <c r="E102" s="59" t="s">
         <v>739</v>
       </c>
     </row>
     <row r="103" spans="2:5" ht="15" customHeight="1">
-      <c r="B103" s="108" t="s">
+      <c r="B103" s="109" t="s">
         <v>782</v>
       </c>
-      <c r="C103" s="108"/>
+      <c r="C103" s="109"/>
       <c r="D103" s="44"/>
-      <c r="E103" s="60"/>
+      <c r="E103" s="59"/>
     </row>
     <row r="104" spans="2:5" ht="45">
-      <c r="B104" s="60" t="s">
+      <c r="B104" s="59" t="s">
         <v>26</v>
       </c>
       <c r="D104" s="44" t="s">
         <v>783</v>
       </c>
-      <c r="E104" s="60" t="s">
+      <c r="E104" s="59" t="s">
         <v>784</v>
       </c>
     </row>
     <row r="105" spans="2:5">
-      <c r="B105" s="60"/>
+      <c r="B105" s="59"/>
       <c r="D105" s="44"/>
-      <c r="E105" s="60"/>
+      <c r="E105" s="59"/>
     </row>
     <row r="106" spans="2:5">
-      <c r="B106" s="108" t="s">
+      <c r="B106" s="109" t="s">
         <v>787</v>
       </c>
-      <c r="C106" s="108"/>
+      <c r="C106" s="109"/>
       <c r="D106" s="44"/>
-      <c r="E106" s="60"/>
+      <c r="E106" s="59"/>
     </row>
     <row r="107" spans="2:5" ht="30">
-      <c r="B107" s="60" t="s">
+      <c r="B107" s="59" t="s">
         <v>26</v>
       </c>
       <c r="D107" s="44" t="s">
         <v>788</v>
       </c>
-      <c r="E107" s="60" t="s">
+      <c r="E107" s="59" t="s">
         <v>789</v>
       </c>
     </row>
     <row r="108" spans="2:5">
-      <c r="B108" s="60"/>
+      <c r="B108" s="59"/>
       <c r="D108" s="44"/>
-      <c r="E108" s="60"/>
+      <c r="E108" s="59"/>
     </row>
     <row r="109" spans="2:5">
-      <c r="B109" s="108" t="s">
+      <c r="B109" s="109" t="s">
         <v>795</v>
       </c>
-      <c r="C109" s="108"/>
-      <c r="E109" s="60"/>
+      <c r="C109" s="109"/>
+      <c r="E109" s="59"/>
     </row>
     <row r="110" spans="2:5" ht="30">
-      <c r="B110" s="60" t="s">
+      <c r="B110" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C110" s="78" t="s">
+      <c r="C110" s="77" t="s">
         <v>798</v>
       </c>
-      <c r="D110" s="79" t="s">
+      <c r="D110" s="78" t="s">
         <v>801</v>
       </c>
-      <c r="E110" s="60" t="s">
+      <c r="E110" s="59" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="111" spans="2:5" ht="45">
-      <c r="B111" s="60"/>
-      <c r="D111" s="80" t="s">
+      <c r="B111" s="59"/>
+      <c r="D111" s="79" t="s">
         <v>796</v>
       </c>
     </row>
     <row r="112" spans="2:5" ht="45">
-      <c r="B112" s="60"/>
+      <c r="B112" s="59"/>
       <c r="D112" s="44" t="s">
         <v>804</v>
       </c>
-      <c r="E112" s="60" t="s">
+      <c r="E112" s="59" t="s">
         <v>799</v>
       </c>
     </row>
     <row r="113" spans="1:1087" ht="90">
-      <c r="B113" s="60"/>
-      <c r="C113" s="78" t="s">
+      <c r="B113" s="59"/>
+      <c r="C113" s="77" t="s">
         <v>797</v>
       </c>
-      <c r="D113" s="79" t="s">
+      <c r="D113" s="78" t="s">
         <v>802</v>
       </c>
-      <c r="E113" s="60" t="s">
+      <c r="E113" s="59" t="s">
         <v>799</v>
       </c>
     </row>
     <row r="114" spans="1:1087" ht="75">
-      <c r="B114" s="60"/>
+      <c r="B114" s="59"/>
       <c r="D114" s="44" t="s">
         <v>803</v>
       </c>
-      <c r="E114" s="60" t="s">
+      <c r="E114" s="59" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="115" spans="1:1087">
-      <c r="B115" s="60"/>
+      <c r="B115" s="59"/>
       <c r="D115" s="44"/>
-      <c r="E115" s="60"/>
+      <c r="E115" s="59"/>
     </row>
     <row r="116" spans="1:1087">
-      <c r="B116" s="108" t="s">
+      <c r="B116" s="109" t="s">
         <v>817</v>
       </c>
-      <c r="C116" s="108"/>
+      <c r="C116" s="109"/>
       <c r="D116" s="44"/>
-      <c r="E116" s="60"/>
+      <c r="E116" s="59"/>
     </row>
     <row r="117" spans="1:1087" ht="45">
-      <c r="B117" s="60" t="s">
+      <c r="B117" s="59" t="s">
         <v>26</v>
       </c>
       <c r="D117" s="44" t="s">
         <v>818</v>
       </c>
-      <c r="E117" s="60" t="s">
+      <c r="E117" s="59" t="s">
         <v>821</v>
       </c>
     </row>
     <row r="118" spans="1:1087">
-      <c r="B118" s="60"/>
+      <c r="B118" s="59"/>
       <c r="D118" s="44"/>
-      <c r="E118" s="60"/>
+      <c r="E118" s="59"/>
     </row>
     <row r="119" spans="1:1087">
-      <c r="B119" s="108" t="s">
+      <c r="B119" s="109" t="s">
         <v>826</v>
       </c>
-      <c r="C119" s="108"/>
+      <c r="C119" s="109"/>
       <c r="D119" s="44"/>
-      <c r="E119" s="60"/>
+      <c r="E119" s="59"/>
     </row>
     <row r="120" spans="1:1087" ht="30">
-      <c r="B120" s="60" t="s">
+      <c r="B120" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C120" s="78" t="s">
+      <c r="C120" s="77" t="s">
         <v>827</v>
       </c>
       <c r="D120" s="44" t="s">
         <v>840</v>
       </c>
-      <c r="E120" s="60" t="s">
+      <c r="E120" s="59" t="s">
         <v>828</v>
       </c>
     </row>
     <row r="121" spans="1:1087">
-      <c r="B121" s="60"/>
+      <c r="B121" s="59"/>
       <c r="D121" s="44"/>
-      <c r="E121" s="60"/>
+      <c r="E121" s="59"/>
     </row>
     <row r="122" spans="1:1087" ht="45">
-      <c r="B122" s="60" t="s">
+      <c r="B122" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C122" s="78" t="s">
+      <c r="C122" s="77" t="s">
         <v>829</v>
       </c>
       <c r="D122" s="44" t="s">
         <v>841</v>
       </c>
-      <c r="E122" s="60" t="s">
+      <c r="E122" s="59" t="s">
         <v>828</v>
       </c>
     </row>
     <row r="123" spans="1:1087">
-      <c r="B123" s="60"/>
+      <c r="B123" s="59"/>
       <c r="D123" s="44"/>
-      <c r="E123" s="60"/>
+      <c r="E123" s="59"/>
     </row>
     <row r="124" spans="1:1087">
       <c r="A124" s="31"/>

</xml_diff>

<commit_message>
Added Rate and Share cases
</commit_message>
<xml_diff>
--- a/Mobile/Manual/Unified Mobile Functional Test Template .xlsx
+++ b/Mobile/Manual/Unified Mobile Functional Test Template .xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="857">
   <si>
     <t>Test date:</t>
   </si>
@@ -5378,9 +5378,6 @@
     <t>8.2 iPhone built-in music controls</t>
   </si>
   <si>
-    <t>8.3 Rate app</t>
-  </si>
-  <si>
     <t>Rate app</t>
   </si>
   <si>
@@ -5390,6 +5387,24 @@
   </si>
   <si>
     <t>The Store app should open on the correct app page</t>
+  </si>
+  <si>
+    <t>8.3 Rate and Share app</t>
+  </si>
+  <si>
+    <t>Share app</t>
+  </si>
+  <si>
+    <t>Reinstall the app and Repeat the above test for Twitter</t>
+  </si>
+  <si>
+    <t>[1] Reinstall the app and Repeat the above test for Email
+[2] Click the picture in the Email on the device</t>
+  </si>
+  <si>
+    <t>[1] Cold start the app up to 5 times until Share screen appears
+[2] Click Facebook
+[3] Sign in and Follow link posted</t>
   </si>
 </sst>
 </file>
@@ -7348,7 +7363,7 @@
   <dimension ref="A1:AMK73"/>
   <sheetViews>
     <sheetView topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8380,16 +8395,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B56:C56"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B56:C56"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70833333333333304" right="1.1000000000000001" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -8401,8 +8416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK84"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9575,17 +9590,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A84:C84"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B61:C61"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70833333333333304" right="1.1000000000000001" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -10824,11 +10839,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="B62:C62"/>
@@ -10839,6 +10849,11 @@
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B53:C53"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70833333333333304" right="1.1000000000000001" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -13813,11 +13828,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="B121:C121"/>
     <mergeCell ref="B142:C142"/>
     <mergeCell ref="B157:C157"/>
@@ -13827,6 +13837,11 @@
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B106:C106"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70833333333333304" right="1.1000000000000001" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -81655,11 +81670,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="B105:C105"/>
     <mergeCell ref="B120:C120"/>
     <mergeCell ref="A140:C140"/>
@@ -81668,6 +81678,11 @@
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B89:C89"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70833333333333304" right="1.1000000000000001" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -83811,11 +83826,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:E6"/>
     <mergeCell ref="B105:C105"/>
     <mergeCell ref="B120:C120"/>
     <mergeCell ref="A141:C141"/>
@@ -83824,6 +83834,11 @@
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B89:C89"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:E6"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70833333333333304" right="1.1000000000000001" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -83833,10 +83848,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AOU127"/>
+  <dimension ref="A1:AOU131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J134" sqref="J134"/>
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -85687,7 +85702,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="113" spans="1:1087" ht="90">
+    <row r="113" spans="2:5" ht="90">
       <c r="B113" s="59"/>
       <c r="C113" s="77" t="s">
         <v>790</v>
@@ -85699,7 +85714,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="114" spans="1:1087" ht="75">
+    <row r="114" spans="2:5" ht="75">
       <c r="B114" s="59"/>
       <c r="D114" s="44" t="s">
         <v>796</v>
@@ -85708,12 +85723,12 @@
         <v>793</v>
       </c>
     </row>
-    <row r="115" spans="1:1087">
+    <row r="115" spans="2:5">
       <c r="B115" s="59"/>
       <c r="D115" s="44"/>
       <c r="E115" s="59"/>
     </row>
-    <row r="116" spans="1:1087">
+    <row r="116" spans="2:5">
       <c r="B116" s="108" t="s">
         <v>810</v>
       </c>
@@ -85721,7 +85736,7 @@
       <c r="D116" s="44"/>
       <c r="E116" s="59"/>
     </row>
-    <row r="117" spans="1:1087" ht="45">
+    <row r="117" spans="2:5" ht="45">
       <c r="B117" s="59" t="s">
         <v>26</v>
       </c>
@@ -85732,12 +85747,12 @@
         <v>814</v>
       </c>
     </row>
-    <row r="118" spans="1:1087">
+    <row r="118" spans="2:5">
       <c r="B118" s="59"/>
       <c r="D118" s="44"/>
       <c r="E118" s="59"/>
     </row>
-    <row r="119" spans="1:1087">
+    <row r="119" spans="2:5">
       <c r="B119" s="108" t="s">
         <v>848</v>
       </c>
@@ -85745,7 +85760,7 @@
       <c r="D119" s="44"/>
       <c r="E119" s="59"/>
     </row>
-    <row r="120" spans="1:1087" ht="30">
+    <row r="120" spans="2:5" ht="30">
       <c r="B120" s="59" t="s">
         <v>42</v>
       </c>
@@ -85759,12 +85774,12 @@
         <v>820</v>
       </c>
     </row>
-    <row r="121" spans="1:1087">
+    <row r="121" spans="2:5">
       <c r="B121" s="59"/>
       <c r="D121" s="44"/>
       <c r="E121" s="59"/>
     </row>
-    <row r="122" spans="1:1087" ht="45">
+    <row r="122" spans="2:5" ht="45">
       <c r="B122" s="59" t="s">
         <v>42</v>
       </c>
@@ -85778,1130 +85793,1176 @@
         <v>820</v>
       </c>
     </row>
-    <row r="123" spans="1:1087">
+    <row r="123" spans="2:5">
       <c r="B123" s="59"/>
       <c r="C123" s="44"/>
       <c r="D123" s="44"/>
       <c r="E123" s="59"/>
     </row>
-    <row r="124" spans="1:1087">
+    <row r="124" spans="2:5">
       <c r="B124" s="108" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="C124" s="108"/>
       <c r="D124" s="44"/>
       <c r="E124" s="59"/>
     </row>
-    <row r="125" spans="1:1087" ht="45">
+    <row r="125" spans="2:5" ht="45">
       <c r="B125" s="59" t="s">
         <v>26</v>
       </c>
       <c r="C125" s="77" t="s">
+        <v>849</v>
+      </c>
+      <c r="D125" s="44" t="s">
         <v>850</v>
       </c>
-      <c r="D125" s="44" t="s">
+      <c r="E125" s="59" t="s">
         <v>851</v>
       </c>
-      <c r="E125" s="59" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1087">
+    </row>
+    <row r="126" spans="2:5">
       <c r="B126" s="59"/>
       <c r="D126" s="44"/>
       <c r="E126" s="59"/>
     </row>
-    <row r="127" spans="1:1087">
-      <c r="A127" s="31"/>
-      <c r="B127" s="31"/>
-      <c r="C127" s="31"/>
-      <c r="D127" s="31"/>
-      <c r="E127" s="31"/>
-      <c r="F127" s="31"/>
-      <c r="G127" s="31"/>
-      <c r="H127" s="31"/>
-      <c r="I127" s="31"/>
-      <c r="J127" s="31"/>
-      <c r="K127" s="31"/>
-      <c r="L127" s="31"/>
-      <c r="M127" s="31"/>
-      <c r="N127" s="31"/>
-      <c r="O127" s="31"/>
-      <c r="P127" s="31"/>
-      <c r="Q127" s="31"/>
-      <c r="R127" s="31"/>
-      <c r="S127" s="31"/>
-      <c r="T127" s="31"/>
-      <c r="U127" s="31"/>
-      <c r="V127" s="31"/>
-      <c r="W127" s="31"/>
-      <c r="X127" s="31"/>
-      <c r="Y127" s="31"/>
-      <c r="Z127" s="31"/>
-      <c r="AA127" s="31"/>
-      <c r="AB127" s="31"/>
-      <c r="AC127" s="31"/>
-      <c r="AD127" s="31"/>
-      <c r="AE127" s="31"/>
-      <c r="AF127" s="31"/>
-      <c r="AG127" s="31"/>
-      <c r="AH127" s="31"/>
-      <c r="AI127" s="31"/>
-      <c r="AJ127" s="31"/>
-      <c r="AK127" s="31"/>
-      <c r="AL127" s="31"/>
-      <c r="AM127" s="31"/>
-      <c r="AN127" s="31"/>
-      <c r="AO127" s="31"/>
-      <c r="AP127" s="31"/>
-      <c r="AQ127" s="31"/>
-      <c r="AR127" s="31"/>
-      <c r="AS127" s="31"/>
-      <c r="AT127" s="31"/>
-      <c r="AU127" s="31"/>
-      <c r="AV127" s="31"/>
-      <c r="AW127" s="31"/>
-      <c r="AX127" s="31"/>
-      <c r="AY127" s="31"/>
-      <c r="AZ127" s="31"/>
-      <c r="BA127" s="31"/>
-      <c r="BB127" s="31"/>
-      <c r="BC127" s="31"/>
-      <c r="BD127" s="31"/>
-      <c r="BE127" s="31"/>
-      <c r="BF127" s="31"/>
-      <c r="BG127" s="31"/>
-      <c r="BH127" s="31"/>
-      <c r="BI127" s="31"/>
-      <c r="BJ127" s="31"/>
-      <c r="BK127" s="31"/>
-      <c r="BL127" s="31"/>
-      <c r="BM127" s="31"/>
-      <c r="BN127" s="31"/>
-      <c r="BO127" s="31"/>
-      <c r="BP127" s="31"/>
-      <c r="BQ127" s="31"/>
-      <c r="BR127" s="31"/>
-      <c r="BS127" s="31"/>
-      <c r="BT127" s="31"/>
-      <c r="BU127" s="31"/>
-      <c r="BV127" s="31"/>
-      <c r="BW127" s="31"/>
-      <c r="BX127" s="31"/>
-      <c r="BY127" s="31"/>
-      <c r="BZ127" s="31"/>
-      <c r="CA127" s="31"/>
-      <c r="CB127" s="31"/>
-      <c r="CC127" s="31"/>
-      <c r="CD127" s="31"/>
-      <c r="CE127" s="31"/>
-      <c r="CF127" s="31"/>
-      <c r="CG127" s="31"/>
-      <c r="CH127" s="31"/>
-      <c r="CI127" s="31"/>
-      <c r="CJ127" s="31"/>
-      <c r="CK127" s="31"/>
-      <c r="CL127" s="31"/>
-      <c r="CM127" s="31"/>
-      <c r="CN127" s="31"/>
-      <c r="CO127" s="31"/>
-      <c r="CP127" s="31"/>
-      <c r="CQ127" s="31"/>
-      <c r="CR127" s="31"/>
-      <c r="CS127" s="31"/>
-      <c r="CT127" s="31"/>
-      <c r="CU127" s="31"/>
-      <c r="CV127" s="31"/>
-      <c r="CW127" s="31"/>
-      <c r="CX127" s="31"/>
-      <c r="CY127" s="31"/>
-      <c r="CZ127" s="31"/>
-      <c r="DA127" s="31"/>
-      <c r="DB127" s="31"/>
-      <c r="DC127" s="31"/>
-      <c r="DD127" s="31"/>
-      <c r="DE127" s="31"/>
-      <c r="DF127" s="31"/>
-      <c r="DG127" s="31"/>
-      <c r="DH127" s="31"/>
-      <c r="DI127" s="31"/>
-      <c r="DJ127" s="31"/>
-      <c r="DK127" s="31"/>
-      <c r="DL127" s="31"/>
-      <c r="DM127" s="31"/>
-      <c r="DN127" s="31"/>
-      <c r="DO127" s="31"/>
-      <c r="DP127" s="31"/>
-      <c r="DQ127" s="31"/>
-      <c r="DR127" s="31"/>
-      <c r="DS127" s="31"/>
-      <c r="DT127" s="31"/>
-      <c r="DU127" s="31"/>
-      <c r="DV127" s="31"/>
-      <c r="DW127" s="31"/>
-      <c r="DX127" s="31"/>
-      <c r="DY127" s="31"/>
-      <c r="DZ127" s="31"/>
-      <c r="EA127" s="31"/>
-      <c r="EB127" s="31"/>
-      <c r="EC127" s="31"/>
-      <c r="ED127" s="31"/>
-      <c r="EE127" s="31"/>
-      <c r="EF127" s="31"/>
-      <c r="EG127" s="31"/>
-      <c r="EH127" s="31"/>
-      <c r="EI127" s="31"/>
-      <c r="EJ127" s="31"/>
-      <c r="EK127" s="31"/>
-      <c r="EL127" s="31"/>
-      <c r="EM127" s="31"/>
-      <c r="EN127" s="31"/>
-      <c r="EO127" s="31"/>
-      <c r="EP127" s="31"/>
-      <c r="EQ127" s="31"/>
-      <c r="ER127" s="31"/>
-      <c r="ES127" s="31"/>
-      <c r="ET127" s="31"/>
-      <c r="EU127" s="31"/>
-      <c r="EV127" s="31"/>
-      <c r="EW127" s="31"/>
-      <c r="EX127" s="31"/>
-      <c r="EY127" s="31"/>
-      <c r="EZ127" s="31"/>
-      <c r="FA127" s="31"/>
-      <c r="FB127" s="31"/>
-      <c r="FC127" s="31"/>
-      <c r="FD127" s="31"/>
-      <c r="FE127" s="31"/>
-      <c r="FF127" s="31"/>
-      <c r="FG127" s="31"/>
-      <c r="FH127" s="31"/>
-      <c r="FI127" s="31"/>
-      <c r="FJ127" s="31"/>
-      <c r="FK127" s="31"/>
-      <c r="FL127" s="31"/>
-      <c r="FM127" s="31"/>
-      <c r="FN127" s="31"/>
-      <c r="FO127" s="31"/>
-      <c r="FP127" s="31"/>
-      <c r="FQ127" s="31"/>
-      <c r="FR127" s="31"/>
-      <c r="FS127" s="31"/>
-      <c r="FT127" s="31"/>
-      <c r="FU127" s="31"/>
-      <c r="FV127" s="31"/>
-      <c r="FW127" s="31"/>
-      <c r="FX127" s="31"/>
-      <c r="FY127" s="31"/>
-      <c r="FZ127" s="31"/>
-      <c r="GA127" s="31"/>
-      <c r="GB127" s="31"/>
-      <c r="GC127" s="31"/>
-      <c r="GD127" s="31"/>
-      <c r="GE127" s="31"/>
-      <c r="GF127" s="31"/>
-      <c r="GG127" s="31"/>
-      <c r="GH127" s="31"/>
-      <c r="GI127" s="31"/>
-      <c r="GJ127" s="31"/>
-      <c r="GK127" s="31"/>
-      <c r="GL127" s="31"/>
-      <c r="GM127" s="31"/>
-      <c r="GN127" s="31"/>
-      <c r="GO127" s="31"/>
-      <c r="GP127" s="31"/>
-      <c r="GQ127" s="31"/>
-      <c r="GR127" s="31"/>
-      <c r="GS127" s="31"/>
-      <c r="GT127" s="31"/>
-      <c r="GU127" s="31"/>
-      <c r="GV127" s="31"/>
-      <c r="GW127" s="31"/>
-      <c r="GX127" s="31"/>
-      <c r="GY127" s="31"/>
-      <c r="GZ127" s="31"/>
-      <c r="HA127" s="31"/>
-      <c r="HB127" s="31"/>
-      <c r="HC127" s="31"/>
-      <c r="HD127" s="31"/>
-      <c r="HE127" s="31"/>
-      <c r="HF127" s="31"/>
-      <c r="HG127" s="31"/>
-      <c r="HH127" s="31"/>
-      <c r="HI127" s="31"/>
-      <c r="HJ127" s="31"/>
-      <c r="HK127" s="31"/>
-      <c r="HL127" s="31"/>
-      <c r="HM127" s="31"/>
-      <c r="HN127" s="31"/>
-      <c r="HO127" s="31"/>
-      <c r="HP127" s="31"/>
-      <c r="HQ127" s="31"/>
-      <c r="HR127" s="31"/>
-      <c r="HS127" s="31"/>
-      <c r="HT127" s="31"/>
-      <c r="HU127" s="31"/>
-      <c r="HV127" s="31"/>
-      <c r="HW127" s="31"/>
-      <c r="HX127" s="31"/>
-      <c r="HY127" s="31"/>
-      <c r="HZ127" s="31"/>
-      <c r="IA127" s="31"/>
-      <c r="IB127" s="31"/>
-      <c r="IC127" s="31"/>
-      <c r="ID127" s="31"/>
-      <c r="IE127" s="31"/>
-      <c r="IF127" s="31"/>
-      <c r="IG127" s="31"/>
-      <c r="IH127" s="31"/>
-      <c r="II127" s="31"/>
-      <c r="IJ127" s="31"/>
-      <c r="IK127" s="31"/>
-      <c r="IL127" s="31"/>
-      <c r="IM127" s="31"/>
-      <c r="IN127" s="31"/>
-      <c r="IO127" s="31"/>
-      <c r="IP127" s="31"/>
-      <c r="IQ127" s="31"/>
-      <c r="IR127" s="31"/>
-      <c r="IS127" s="31"/>
-      <c r="IT127" s="31"/>
-      <c r="IU127" s="31"/>
-      <c r="IV127" s="31"/>
-      <c r="IW127" s="31"/>
-      <c r="IX127" s="31"/>
-      <c r="IY127" s="31"/>
-      <c r="IZ127" s="31"/>
-      <c r="JA127" s="31"/>
-      <c r="JB127" s="31"/>
-      <c r="JC127" s="31"/>
-      <c r="JD127" s="31"/>
-      <c r="JE127" s="31"/>
-      <c r="JF127" s="31"/>
-      <c r="JG127" s="31"/>
-      <c r="JH127" s="31"/>
-      <c r="JI127" s="31"/>
-      <c r="JJ127" s="31"/>
-      <c r="JK127" s="31"/>
-      <c r="JL127" s="31"/>
-      <c r="JM127" s="31"/>
-      <c r="JN127" s="31"/>
-      <c r="JO127" s="31"/>
-      <c r="JP127" s="31"/>
-      <c r="JQ127" s="31"/>
-      <c r="JR127" s="31"/>
-      <c r="JS127" s="31"/>
-      <c r="JT127" s="31"/>
-      <c r="JU127" s="31"/>
-      <c r="JV127" s="31"/>
-      <c r="JW127" s="31"/>
-      <c r="JX127" s="31"/>
-      <c r="JY127" s="31"/>
-      <c r="JZ127" s="31"/>
-      <c r="KA127" s="31"/>
-      <c r="KB127" s="31"/>
-      <c r="KC127" s="31"/>
-      <c r="KD127" s="31"/>
-      <c r="KE127" s="31"/>
-      <c r="KF127" s="31"/>
-      <c r="KG127" s="31"/>
-      <c r="KH127" s="31"/>
-      <c r="KI127" s="31"/>
-      <c r="KJ127" s="31"/>
-      <c r="KK127" s="31"/>
-      <c r="KL127" s="31"/>
-      <c r="KM127" s="31"/>
-      <c r="KN127" s="31"/>
-      <c r="KO127" s="31"/>
-      <c r="KP127" s="31"/>
-      <c r="KQ127" s="31"/>
-      <c r="KR127" s="31"/>
-      <c r="KS127" s="31"/>
-      <c r="KT127" s="31"/>
-      <c r="KU127" s="31"/>
-      <c r="KV127" s="31"/>
-      <c r="KW127" s="31"/>
-      <c r="KX127" s="31"/>
-      <c r="KY127" s="31"/>
-      <c r="KZ127" s="31"/>
-      <c r="LA127" s="31"/>
-      <c r="LB127" s="31"/>
-      <c r="LC127" s="31"/>
-      <c r="LD127" s="31"/>
-      <c r="LE127" s="31"/>
-      <c r="LF127" s="31"/>
-      <c r="LG127" s="31"/>
-      <c r="LH127" s="31"/>
-      <c r="LI127" s="31"/>
-      <c r="LJ127" s="31"/>
-      <c r="LK127" s="31"/>
-      <c r="LL127" s="31"/>
-      <c r="LM127" s="31"/>
-      <c r="LN127" s="31"/>
-      <c r="LO127" s="31"/>
-      <c r="LP127" s="31"/>
-      <c r="LQ127" s="31"/>
-      <c r="LR127" s="31"/>
-      <c r="LS127" s="31"/>
-      <c r="LT127" s="31"/>
-      <c r="LU127" s="31"/>
-      <c r="LV127" s="31"/>
-      <c r="LW127" s="31"/>
-      <c r="LX127" s="31"/>
-      <c r="LY127" s="31"/>
-      <c r="LZ127" s="31"/>
-      <c r="MA127" s="31"/>
-      <c r="MB127" s="31"/>
-      <c r="MC127" s="31"/>
-      <c r="MD127" s="31"/>
-      <c r="ME127" s="31"/>
-      <c r="MF127" s="31"/>
-      <c r="MG127" s="31"/>
-      <c r="MH127" s="31"/>
-      <c r="MI127" s="31"/>
-      <c r="MJ127" s="31"/>
-      <c r="MK127" s="31"/>
-      <c r="ML127" s="31"/>
-      <c r="MM127" s="31"/>
-      <c r="MN127" s="31"/>
-      <c r="MO127" s="31"/>
-      <c r="MP127" s="31"/>
-      <c r="MQ127" s="31"/>
-      <c r="MR127" s="31"/>
-      <c r="MS127" s="31"/>
-      <c r="MT127" s="31"/>
-      <c r="MU127" s="31"/>
-      <c r="MV127" s="31"/>
-      <c r="MW127" s="31"/>
-      <c r="MX127" s="31"/>
-      <c r="MY127" s="31"/>
-      <c r="MZ127" s="31"/>
-      <c r="NA127" s="31"/>
-      <c r="NB127" s="31"/>
-      <c r="NC127" s="31"/>
-      <c r="ND127" s="31"/>
-      <c r="NE127" s="31"/>
-      <c r="NF127" s="31"/>
-      <c r="NG127" s="31"/>
-      <c r="NH127" s="31"/>
-      <c r="NI127" s="31"/>
-      <c r="NJ127" s="31"/>
-      <c r="NK127" s="31"/>
-      <c r="NL127" s="31"/>
-      <c r="NM127" s="31"/>
-      <c r="NN127" s="31"/>
-      <c r="NO127" s="31"/>
-      <c r="NP127" s="31"/>
-      <c r="NQ127" s="31"/>
-      <c r="NR127" s="31"/>
-      <c r="NS127" s="31"/>
-      <c r="NT127" s="31"/>
-      <c r="NU127" s="31"/>
-      <c r="NV127" s="31"/>
-      <c r="NW127" s="31"/>
-      <c r="NX127" s="31"/>
-      <c r="NY127" s="31"/>
-      <c r="NZ127" s="31"/>
-      <c r="OA127" s="31"/>
-      <c r="OB127" s="31"/>
-      <c r="OC127" s="31"/>
-      <c r="OD127" s="31"/>
-      <c r="OE127" s="31"/>
-      <c r="OF127" s="31"/>
-      <c r="OG127" s="31"/>
-      <c r="OH127" s="31"/>
-      <c r="OI127" s="31"/>
-      <c r="OJ127" s="31"/>
-      <c r="OK127" s="31"/>
-      <c r="OL127" s="31"/>
-      <c r="OM127" s="31"/>
-      <c r="ON127" s="31"/>
-      <c r="OO127" s="31"/>
-      <c r="OP127" s="31"/>
-      <c r="OQ127" s="31"/>
-      <c r="OR127" s="31"/>
-      <c r="OS127" s="31"/>
-      <c r="OT127" s="31"/>
-      <c r="OU127" s="31"/>
-      <c r="OV127" s="31"/>
-      <c r="OW127" s="31"/>
-      <c r="OX127" s="31"/>
-      <c r="OY127" s="31"/>
-      <c r="OZ127" s="31"/>
-      <c r="PA127" s="31"/>
-      <c r="PB127" s="31"/>
-      <c r="PC127" s="31"/>
-      <c r="PD127" s="31"/>
-      <c r="PE127" s="31"/>
-      <c r="PF127" s="31"/>
-      <c r="PG127" s="31"/>
-      <c r="PH127" s="31"/>
-      <c r="PI127" s="31"/>
-      <c r="PJ127" s="31"/>
-      <c r="PK127" s="31"/>
-      <c r="PL127" s="31"/>
-      <c r="PM127" s="31"/>
-      <c r="PN127" s="31"/>
-      <c r="PO127" s="31"/>
-      <c r="PP127" s="31"/>
-      <c r="PQ127" s="31"/>
-      <c r="PR127" s="31"/>
-      <c r="PS127" s="31"/>
-      <c r="PT127" s="31"/>
-      <c r="PU127" s="31"/>
-      <c r="PV127" s="31"/>
-      <c r="PW127" s="31"/>
-      <c r="PX127" s="31"/>
-      <c r="PY127" s="31"/>
-      <c r="PZ127" s="31"/>
-      <c r="QA127" s="31"/>
-      <c r="QB127" s="31"/>
-      <c r="QC127" s="31"/>
-      <c r="QD127" s="31"/>
-      <c r="QE127" s="31"/>
-      <c r="QF127" s="31"/>
-      <c r="QG127" s="31"/>
-      <c r="QH127" s="31"/>
-      <c r="QI127" s="31"/>
-      <c r="QJ127" s="31"/>
-      <c r="QK127" s="31"/>
-      <c r="QL127" s="31"/>
-      <c r="QM127" s="31"/>
-      <c r="QN127" s="31"/>
-      <c r="QO127" s="31"/>
-      <c r="QP127" s="31"/>
-      <c r="QQ127" s="31"/>
-      <c r="QR127" s="31"/>
-      <c r="QS127" s="31"/>
-      <c r="QT127" s="31"/>
-      <c r="QU127" s="31"/>
-      <c r="QV127" s="31"/>
-      <c r="QW127" s="31"/>
-      <c r="QX127" s="31"/>
-      <c r="QY127" s="31"/>
-      <c r="QZ127" s="31"/>
-      <c r="RA127" s="31"/>
-      <c r="RB127" s="31"/>
-      <c r="RC127" s="31"/>
-      <c r="RD127" s="31"/>
-      <c r="RE127" s="31"/>
-      <c r="RF127" s="31"/>
-      <c r="RG127" s="31"/>
-      <c r="RH127" s="31"/>
-      <c r="RI127" s="31"/>
-      <c r="RJ127" s="31"/>
-      <c r="RK127" s="31"/>
-      <c r="RL127" s="31"/>
-      <c r="RM127" s="31"/>
-      <c r="RN127" s="31"/>
-      <c r="RO127" s="31"/>
-      <c r="RP127" s="31"/>
-      <c r="RQ127" s="31"/>
-      <c r="RR127" s="31"/>
-      <c r="RS127" s="31"/>
-      <c r="RT127" s="31"/>
-      <c r="RU127" s="31"/>
-      <c r="RV127" s="31"/>
-      <c r="RW127" s="31"/>
-      <c r="RX127" s="31"/>
-      <c r="RY127" s="31"/>
-      <c r="RZ127" s="31"/>
-      <c r="SA127" s="31"/>
-      <c r="SB127" s="31"/>
-      <c r="SC127" s="31"/>
-      <c r="SD127" s="31"/>
-      <c r="SE127" s="31"/>
-      <c r="SF127" s="31"/>
-      <c r="SG127" s="31"/>
-      <c r="SH127" s="31"/>
-      <c r="SI127" s="31"/>
-      <c r="SJ127" s="31"/>
-      <c r="SK127" s="31"/>
-      <c r="SL127" s="31"/>
-      <c r="SM127" s="31"/>
-      <c r="SN127" s="31"/>
-      <c r="SO127" s="31"/>
-      <c r="SP127" s="31"/>
-      <c r="SQ127" s="31"/>
-      <c r="SR127" s="31"/>
-      <c r="SS127" s="31"/>
-      <c r="ST127" s="31"/>
-      <c r="SU127" s="31"/>
-      <c r="SV127" s="31"/>
-      <c r="SW127" s="31"/>
-      <c r="SX127" s="31"/>
-      <c r="SY127" s="31"/>
-      <c r="SZ127" s="31"/>
-      <c r="TA127" s="31"/>
-      <c r="TB127" s="31"/>
-      <c r="TC127" s="31"/>
-      <c r="TD127" s="31"/>
-      <c r="TE127" s="31"/>
-      <c r="TF127" s="31"/>
-      <c r="TG127" s="31"/>
-      <c r="TH127" s="31"/>
-      <c r="TI127" s="31"/>
-      <c r="TJ127" s="31"/>
-      <c r="TK127" s="31"/>
-      <c r="TL127" s="31"/>
-      <c r="TM127" s="31"/>
-      <c r="TN127" s="31"/>
-      <c r="TO127" s="31"/>
-      <c r="TP127" s="31"/>
-      <c r="TQ127" s="31"/>
-      <c r="TR127" s="31"/>
-      <c r="TS127" s="31"/>
-      <c r="TT127" s="31"/>
-      <c r="TU127" s="31"/>
-      <c r="TV127" s="31"/>
-      <c r="TW127" s="31"/>
-      <c r="TX127" s="31"/>
-      <c r="TY127" s="31"/>
-      <c r="TZ127" s="31"/>
-      <c r="UA127" s="31"/>
-      <c r="UB127" s="31"/>
-      <c r="UC127" s="31"/>
-      <c r="UD127" s="31"/>
-      <c r="UE127" s="31"/>
-      <c r="UF127" s="31"/>
-      <c r="UG127" s="31"/>
-      <c r="UH127" s="31"/>
-      <c r="UI127" s="31"/>
-      <c r="UJ127" s="31"/>
-      <c r="UK127" s="31"/>
-      <c r="UL127" s="31"/>
-      <c r="UM127" s="31"/>
-      <c r="UN127" s="31"/>
-      <c r="UO127" s="31"/>
-      <c r="UP127" s="31"/>
-      <c r="UQ127" s="31"/>
-      <c r="UR127" s="31"/>
-      <c r="US127" s="31"/>
-      <c r="UT127" s="31"/>
-      <c r="UU127" s="31"/>
-      <c r="UV127" s="31"/>
-      <c r="UW127" s="31"/>
-      <c r="UX127" s="31"/>
-      <c r="UY127" s="31"/>
-      <c r="UZ127" s="31"/>
-      <c r="VA127" s="31"/>
-      <c r="VB127" s="31"/>
-      <c r="VC127" s="31"/>
-      <c r="VD127" s="31"/>
-      <c r="VE127" s="31"/>
-      <c r="VF127" s="31"/>
-      <c r="VG127" s="31"/>
-      <c r="VH127" s="31"/>
-      <c r="VI127" s="31"/>
-      <c r="VJ127" s="31"/>
-      <c r="VK127" s="31"/>
-      <c r="VL127" s="31"/>
-      <c r="VM127" s="31"/>
-      <c r="VN127" s="31"/>
-      <c r="VO127" s="31"/>
-      <c r="VP127" s="31"/>
-      <c r="VQ127" s="31"/>
-      <c r="VR127" s="31"/>
-      <c r="VS127" s="31"/>
-      <c r="VT127" s="31"/>
-      <c r="VU127" s="31"/>
-      <c r="VV127" s="31"/>
-      <c r="VW127" s="31"/>
-      <c r="VX127" s="31"/>
-      <c r="VY127" s="31"/>
-      <c r="VZ127" s="31"/>
-      <c r="WA127" s="31"/>
-      <c r="WB127" s="31"/>
-      <c r="WC127" s="31"/>
-      <c r="WD127" s="31"/>
-      <c r="WE127" s="31"/>
-      <c r="WF127" s="31"/>
-      <c r="WG127" s="31"/>
-      <c r="WH127" s="31"/>
-      <c r="WI127" s="31"/>
-      <c r="WJ127" s="31"/>
-      <c r="WK127" s="31"/>
-      <c r="WL127" s="31"/>
-      <c r="WM127" s="31"/>
-      <c r="WN127" s="31"/>
-      <c r="WO127" s="31"/>
-      <c r="WP127" s="31"/>
-      <c r="WQ127" s="31"/>
-      <c r="WR127" s="31"/>
-      <c r="WS127" s="31"/>
-      <c r="WT127" s="31"/>
-      <c r="WU127" s="31"/>
-      <c r="WV127" s="31"/>
-      <c r="WW127" s="31"/>
-      <c r="WX127" s="31"/>
-      <c r="WY127" s="31"/>
-      <c r="WZ127" s="31"/>
-      <c r="XA127" s="31"/>
-      <c r="XB127" s="31"/>
-      <c r="XC127" s="31"/>
-      <c r="XD127" s="31"/>
-      <c r="XE127" s="31"/>
-      <c r="XF127" s="31"/>
-      <c r="XG127" s="31"/>
-      <c r="XH127" s="31"/>
-      <c r="XI127" s="31"/>
-      <c r="XJ127" s="31"/>
-      <c r="XK127" s="31"/>
-      <c r="XL127" s="31"/>
-      <c r="XM127" s="31"/>
-      <c r="XN127" s="31"/>
-      <c r="XO127" s="31"/>
-      <c r="XP127" s="31"/>
-      <c r="XQ127" s="31"/>
-      <c r="XR127" s="31"/>
-      <c r="XS127" s="31"/>
-      <c r="XT127" s="31"/>
-      <c r="XU127" s="31"/>
-      <c r="XV127" s="31"/>
-      <c r="XW127" s="31"/>
-      <c r="XX127" s="31"/>
-      <c r="XY127" s="31"/>
-      <c r="XZ127" s="31"/>
-      <c r="YA127" s="31"/>
-      <c r="YB127" s="31"/>
-      <c r="YC127" s="31"/>
-      <c r="YD127" s="31"/>
-      <c r="YE127" s="31"/>
-      <c r="YF127" s="31"/>
-      <c r="YG127" s="31"/>
-      <c r="YH127" s="31"/>
-      <c r="YI127" s="31"/>
-      <c r="YJ127" s="31"/>
-      <c r="YK127" s="31"/>
-      <c r="YL127" s="31"/>
-      <c r="YM127" s="31"/>
-      <c r="YN127" s="31"/>
-      <c r="YO127" s="31"/>
-      <c r="YP127" s="31"/>
-      <c r="YQ127" s="31"/>
-      <c r="YR127" s="31"/>
-      <c r="YS127" s="31"/>
-      <c r="YT127" s="31"/>
-      <c r="YU127" s="31"/>
-      <c r="YV127" s="31"/>
-      <c r="YW127" s="31"/>
-      <c r="YX127" s="31"/>
-      <c r="YY127" s="31"/>
-      <c r="YZ127" s="31"/>
-      <c r="ZA127" s="31"/>
-      <c r="ZB127" s="31"/>
-      <c r="ZC127" s="31"/>
-      <c r="ZD127" s="31"/>
-      <c r="ZE127" s="31"/>
-      <c r="ZF127" s="31"/>
-      <c r="ZG127" s="31"/>
-      <c r="ZH127" s="31"/>
-      <c r="ZI127" s="31"/>
-      <c r="ZJ127" s="31"/>
-      <c r="ZK127" s="31"/>
-      <c r="ZL127" s="31"/>
-      <c r="ZM127" s="31"/>
-      <c r="ZN127" s="31"/>
-      <c r="ZO127" s="31"/>
-      <c r="ZP127" s="31"/>
-      <c r="ZQ127" s="31"/>
-      <c r="ZR127" s="31"/>
-      <c r="ZS127" s="31"/>
-      <c r="ZT127" s="31"/>
-      <c r="ZU127" s="31"/>
-      <c r="ZV127" s="31"/>
-      <c r="ZW127" s="31"/>
-      <c r="ZX127" s="31"/>
-      <c r="ZY127" s="31"/>
-      <c r="ZZ127" s="31"/>
-      <c r="AAA127" s="31"/>
-      <c r="AAB127" s="31"/>
-      <c r="AAC127" s="31"/>
-      <c r="AAD127" s="31"/>
-      <c r="AAE127" s="31"/>
-      <c r="AAF127" s="31"/>
-      <c r="AAG127" s="31"/>
-      <c r="AAH127" s="31"/>
-      <c r="AAI127" s="31"/>
-      <c r="AAJ127" s="31"/>
-      <c r="AAK127" s="31"/>
-      <c r="AAL127" s="31"/>
-      <c r="AAM127" s="31"/>
-      <c r="AAN127" s="31"/>
-      <c r="AAO127" s="31"/>
-      <c r="AAP127" s="31"/>
-      <c r="AAQ127" s="31"/>
-      <c r="AAR127" s="31"/>
-      <c r="AAS127" s="31"/>
-      <c r="AAT127" s="31"/>
-      <c r="AAU127" s="31"/>
-      <c r="AAV127" s="31"/>
-      <c r="AAW127" s="31"/>
-      <c r="AAX127" s="31"/>
-      <c r="AAY127" s="31"/>
-      <c r="AAZ127" s="31"/>
-      <c r="ABA127" s="31"/>
-      <c r="ABB127" s="31"/>
-      <c r="ABC127" s="31"/>
-      <c r="ABD127" s="31"/>
-      <c r="ABE127" s="31"/>
-      <c r="ABF127" s="31"/>
-      <c r="ABG127" s="31"/>
-      <c r="ABH127" s="31"/>
-      <c r="ABI127" s="31"/>
-      <c r="ABJ127" s="31"/>
-      <c r="ABK127" s="31"/>
-      <c r="ABL127" s="31"/>
-      <c r="ABM127" s="31"/>
-      <c r="ABN127" s="31"/>
-      <c r="ABO127" s="31"/>
-      <c r="ABP127" s="31"/>
-      <c r="ABQ127" s="31"/>
-      <c r="ABR127" s="31"/>
-      <c r="ABS127" s="31"/>
-      <c r="ABT127" s="31"/>
-      <c r="ABU127" s="31"/>
-      <c r="ABV127" s="31"/>
-      <c r="ABW127" s="31"/>
-      <c r="ABX127" s="31"/>
-      <c r="ABY127" s="31"/>
-      <c r="ABZ127" s="31"/>
-      <c r="ACA127" s="31"/>
-      <c r="ACB127" s="31"/>
-      <c r="ACC127" s="31"/>
-      <c r="ACD127" s="31"/>
-      <c r="ACE127" s="31"/>
-      <c r="ACF127" s="31"/>
-      <c r="ACG127" s="31"/>
-      <c r="ACH127" s="31"/>
-      <c r="ACI127" s="31"/>
-      <c r="ACJ127" s="31"/>
-      <c r="ACK127" s="31"/>
-      <c r="ACL127" s="31"/>
-      <c r="ACM127" s="31"/>
-      <c r="ACN127" s="31"/>
-      <c r="ACO127" s="31"/>
-      <c r="ACP127" s="31"/>
-      <c r="ACQ127" s="31"/>
-      <c r="ACR127" s="31"/>
-      <c r="ACS127" s="31"/>
-      <c r="ACT127" s="31"/>
-      <c r="ACU127" s="31"/>
-      <c r="ACV127" s="31"/>
-      <c r="ACW127" s="31"/>
-      <c r="ACX127" s="31"/>
-      <c r="ACY127" s="31"/>
-      <c r="ACZ127" s="31"/>
-      <c r="ADA127" s="31"/>
-      <c r="ADB127" s="31"/>
-      <c r="ADC127" s="31"/>
-      <c r="ADD127" s="31"/>
-      <c r="ADE127" s="31"/>
-      <c r="ADF127" s="31"/>
-      <c r="ADG127" s="31"/>
-      <c r="ADH127" s="31"/>
-      <c r="ADI127" s="31"/>
-      <c r="ADJ127" s="31"/>
-      <c r="ADK127" s="31"/>
-      <c r="ADL127" s="31"/>
-      <c r="ADM127" s="31"/>
-      <c r="ADN127" s="31"/>
-      <c r="ADO127" s="31"/>
-      <c r="ADP127" s="31"/>
-      <c r="ADQ127" s="31"/>
-      <c r="ADR127" s="31"/>
-      <c r="ADS127" s="31"/>
-      <c r="ADT127" s="31"/>
-      <c r="ADU127" s="31"/>
-      <c r="ADV127" s="31"/>
-      <c r="ADW127" s="31"/>
-      <c r="ADX127" s="31"/>
-      <c r="ADY127" s="31"/>
-      <c r="ADZ127" s="31"/>
-      <c r="AEA127" s="31"/>
-      <c r="AEB127" s="31"/>
-      <c r="AEC127" s="31"/>
-      <c r="AED127" s="31"/>
-      <c r="AEE127" s="31"/>
-      <c r="AEF127" s="31"/>
-      <c r="AEG127" s="31"/>
-      <c r="AEH127" s="31"/>
-      <c r="AEI127" s="31"/>
-      <c r="AEJ127" s="31"/>
-      <c r="AEK127" s="31"/>
-      <c r="AEL127" s="31"/>
-      <c r="AEM127" s="31"/>
-      <c r="AEN127" s="31"/>
-      <c r="AEO127" s="31"/>
-      <c r="AEP127" s="31"/>
-      <c r="AEQ127" s="31"/>
-      <c r="AER127" s="31"/>
-      <c r="AES127" s="31"/>
-      <c r="AET127" s="31"/>
-      <c r="AEU127" s="31"/>
-      <c r="AEV127" s="31"/>
-      <c r="AEW127" s="31"/>
-      <c r="AEX127" s="31"/>
-      <c r="AEY127" s="31"/>
-      <c r="AEZ127" s="31"/>
-      <c r="AFA127" s="31"/>
-      <c r="AFB127" s="31"/>
-      <c r="AFC127" s="31"/>
-      <c r="AFD127" s="31"/>
-      <c r="AFE127" s="31"/>
-      <c r="AFF127" s="31"/>
-      <c r="AFG127" s="31"/>
-      <c r="AFH127" s="31"/>
-      <c r="AFI127" s="31"/>
-      <c r="AFJ127" s="31"/>
-      <c r="AFK127" s="31"/>
-      <c r="AFL127" s="31"/>
-      <c r="AFM127" s="31"/>
-      <c r="AFN127" s="31"/>
-      <c r="AFO127" s="31"/>
-      <c r="AFP127" s="31"/>
-      <c r="AFQ127" s="31"/>
-      <c r="AFR127" s="31"/>
-      <c r="AFS127" s="31"/>
-      <c r="AFT127" s="31"/>
-      <c r="AFU127" s="31"/>
-      <c r="AFV127" s="31"/>
-      <c r="AFW127" s="31"/>
-      <c r="AFX127" s="31"/>
-      <c r="AFY127" s="31"/>
-      <c r="AFZ127" s="31"/>
-      <c r="AGA127" s="31"/>
-      <c r="AGB127" s="31"/>
-      <c r="AGC127" s="31"/>
-      <c r="AGD127" s="31"/>
-      <c r="AGE127" s="31"/>
-      <c r="AGF127" s="31"/>
-      <c r="AGG127" s="31"/>
-      <c r="AGH127" s="31"/>
-      <c r="AGI127" s="31"/>
-      <c r="AGJ127" s="31"/>
-      <c r="AGK127" s="31"/>
-      <c r="AGL127" s="31"/>
-      <c r="AGM127" s="31"/>
-      <c r="AGN127" s="31"/>
-      <c r="AGO127" s="31"/>
-      <c r="AGP127" s="31"/>
-      <c r="AGQ127" s="31"/>
-      <c r="AGR127" s="31"/>
-      <c r="AGS127" s="31"/>
-      <c r="AGT127" s="31"/>
-      <c r="AGU127" s="31"/>
-      <c r="AGV127" s="31"/>
-      <c r="AGW127" s="31"/>
-      <c r="AGX127" s="31"/>
-      <c r="AGY127" s="31"/>
-      <c r="AGZ127" s="31"/>
-      <c r="AHA127" s="31"/>
-      <c r="AHB127" s="31"/>
-      <c r="AHC127" s="31"/>
-      <c r="AHD127" s="31"/>
-      <c r="AHE127" s="31"/>
-      <c r="AHF127" s="31"/>
-      <c r="AHG127" s="31"/>
-      <c r="AHH127" s="31"/>
-      <c r="AHI127" s="31"/>
-      <c r="AHJ127" s="31"/>
-      <c r="AHK127" s="31"/>
-      <c r="AHL127" s="31"/>
-      <c r="AHM127" s="31"/>
-      <c r="AHN127" s="31"/>
-      <c r="AHO127" s="31"/>
-      <c r="AHP127" s="31"/>
-      <c r="AHQ127" s="31"/>
-      <c r="AHR127" s="31"/>
-      <c r="AHS127" s="31"/>
-      <c r="AHT127" s="31"/>
-      <c r="AHU127" s="31"/>
-      <c r="AHV127" s="31"/>
-      <c r="AHW127" s="31"/>
-      <c r="AHX127" s="31"/>
-      <c r="AHY127" s="31"/>
-      <c r="AHZ127" s="31"/>
-      <c r="AIA127" s="31"/>
-      <c r="AIB127" s="31"/>
-      <c r="AIC127" s="31"/>
-      <c r="AID127" s="31"/>
-      <c r="AIE127" s="31"/>
-      <c r="AIF127" s="31"/>
-      <c r="AIG127" s="31"/>
-      <c r="AIH127" s="31"/>
-      <c r="AII127" s="31"/>
-      <c r="AIJ127" s="31"/>
-      <c r="AIK127" s="31"/>
-      <c r="AIL127" s="31"/>
-      <c r="AIM127" s="31"/>
-      <c r="AIN127" s="31"/>
-      <c r="AIO127" s="31"/>
-      <c r="AIP127" s="31"/>
-      <c r="AIQ127" s="31"/>
-      <c r="AIR127" s="31"/>
-      <c r="AIS127" s="31"/>
-      <c r="AIT127" s="31"/>
-      <c r="AIU127" s="31"/>
-      <c r="AIV127" s="31"/>
-      <c r="AIW127" s="31"/>
-      <c r="AIX127" s="31"/>
-      <c r="AIY127" s="31"/>
-      <c r="AIZ127" s="31"/>
-      <c r="AJA127" s="31"/>
-      <c r="AJB127" s="31"/>
-      <c r="AJC127" s="31"/>
-      <c r="AJD127" s="31"/>
-      <c r="AJE127" s="31"/>
-      <c r="AJF127" s="31"/>
-      <c r="AJG127" s="31"/>
-      <c r="AJH127" s="31"/>
-      <c r="AJI127" s="31"/>
-      <c r="AJJ127" s="31"/>
-      <c r="AJK127" s="31"/>
-      <c r="AJL127" s="31"/>
-      <c r="AJM127" s="31"/>
-      <c r="AJN127" s="31"/>
-      <c r="AJO127" s="31"/>
-      <c r="AJP127" s="31"/>
-      <c r="AJQ127" s="31"/>
-      <c r="AJR127" s="31"/>
-      <c r="AJS127" s="31"/>
-      <c r="AJT127" s="31"/>
-      <c r="AJU127" s="31"/>
-      <c r="AJV127" s="31"/>
-      <c r="AJW127" s="31"/>
-      <c r="AJX127" s="31"/>
-      <c r="AJY127" s="31"/>
-      <c r="AJZ127" s="31"/>
-      <c r="AKA127" s="31"/>
-      <c r="AKB127" s="31"/>
-      <c r="AKC127" s="31"/>
-      <c r="AKD127" s="31"/>
-      <c r="AKE127" s="31"/>
-      <c r="AKF127" s="31"/>
-      <c r="AKG127" s="31"/>
-      <c r="AKH127" s="31"/>
-      <c r="AKI127" s="31"/>
-      <c r="AKJ127" s="31"/>
-      <c r="AKK127" s="31"/>
-      <c r="AKL127" s="31"/>
-      <c r="AKM127" s="31"/>
-      <c r="AKN127" s="31"/>
-      <c r="AKO127" s="31"/>
-      <c r="AKP127" s="31"/>
-      <c r="AKQ127" s="31"/>
-      <c r="AKR127" s="31"/>
-      <c r="AKS127" s="31"/>
-      <c r="AKT127" s="31"/>
-      <c r="AKU127" s="31"/>
-      <c r="AKV127" s="31"/>
-      <c r="AKW127" s="31"/>
-      <c r="AKX127" s="31"/>
-      <c r="AKY127" s="31"/>
-      <c r="AKZ127" s="31"/>
-      <c r="ALA127" s="31"/>
-      <c r="ALB127" s="31"/>
-      <c r="ALC127" s="31"/>
-      <c r="ALD127" s="31"/>
-      <c r="ALE127" s="31"/>
-      <c r="ALF127" s="31"/>
-      <c r="ALG127" s="31"/>
-      <c r="ALH127" s="31"/>
-      <c r="ALI127" s="31"/>
-      <c r="ALJ127" s="31"/>
-      <c r="ALK127" s="31"/>
-      <c r="ALL127" s="31"/>
-      <c r="ALM127" s="31"/>
-      <c r="ALN127" s="31"/>
-      <c r="ALO127" s="31"/>
-      <c r="ALP127" s="31"/>
-      <c r="ALQ127" s="31"/>
-      <c r="ALR127" s="31"/>
-      <c r="ALS127" s="31"/>
-      <c r="ALT127" s="31"/>
-      <c r="ALU127" s="31"/>
-      <c r="ALV127" s="31"/>
-      <c r="ALW127" s="31"/>
-      <c r="ALX127" s="31"/>
-      <c r="ALY127" s="31"/>
-      <c r="ALZ127" s="31"/>
-      <c r="AMA127" s="31"/>
-      <c r="AMB127" s="31"/>
-      <c r="AMC127" s="31"/>
-      <c r="AMD127" s="31"/>
-      <c r="AME127" s="31"/>
-      <c r="AMF127" s="31"/>
-      <c r="AMG127" s="31"/>
-      <c r="AMH127" s="31"/>
-      <c r="AMI127" s="31"/>
-      <c r="AMJ127" s="31"/>
-      <c r="AMK127" s="31"/>
-      <c r="AML127" s="31"/>
-      <c r="AMM127" s="31"/>
-      <c r="AMN127" s="31"/>
-      <c r="AMO127" s="31"/>
-      <c r="AMP127" s="31"/>
-      <c r="AMQ127" s="31"/>
-      <c r="AMR127" s="31"/>
-      <c r="AMS127" s="31"/>
-      <c r="AMT127" s="31"/>
-      <c r="AMU127" s="31"/>
-      <c r="AMV127" s="31"/>
-      <c r="AMW127" s="31"/>
-      <c r="AMX127" s="31"/>
-      <c r="AMY127" s="31"/>
-      <c r="AMZ127" s="31"/>
-      <c r="ANA127" s="31"/>
-      <c r="ANB127" s="31"/>
-      <c r="ANC127" s="31"/>
-      <c r="AND127" s="31"/>
-      <c r="ANE127" s="31"/>
-      <c r="ANF127" s="31"/>
-      <c r="ANG127" s="31"/>
-      <c r="ANH127" s="31"/>
-      <c r="ANI127" s="31"/>
-      <c r="ANJ127" s="31"/>
-      <c r="ANK127" s="31"/>
-      <c r="ANL127" s="31"/>
-      <c r="ANM127" s="31"/>
-      <c r="ANN127" s="31"/>
-      <c r="ANO127" s="31"/>
-      <c r="ANP127" s="31"/>
-      <c r="ANQ127" s="31"/>
-      <c r="ANR127" s="31"/>
-      <c r="ANS127" s="31"/>
-      <c r="ANT127" s="31"/>
-      <c r="ANU127" s="31"/>
-      <c r="ANV127" s="31"/>
-      <c r="ANW127" s="31"/>
-      <c r="ANX127" s="31"/>
-      <c r="ANY127" s="31"/>
-      <c r="ANZ127" s="31"/>
-      <c r="AOA127" s="31"/>
-      <c r="AOB127" s="31"/>
-      <c r="AOC127" s="31"/>
-      <c r="AOD127" s="31"/>
-      <c r="AOE127" s="31"/>
-      <c r="AOF127" s="31"/>
-      <c r="AOG127" s="31"/>
-      <c r="AOH127" s="31"/>
-      <c r="AOI127" s="31"/>
-      <c r="AOJ127" s="31"/>
-      <c r="AOK127" s="31"/>
-      <c r="AOL127" s="31"/>
-      <c r="AOM127" s="31"/>
-      <c r="AON127" s="31"/>
-      <c r="AOO127" s="31"/>
-      <c r="AOP127" s="31"/>
-      <c r="AOQ127" s="31"/>
-      <c r="AOR127" s="31"/>
-      <c r="AOS127" s="31"/>
-      <c r="AOT127" s="31"/>
-      <c r="AOU127" s="31"/>
+    <row r="127" spans="2:5" ht="60">
+      <c r="B127" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C127" s="77" t="s">
+        <v>853</v>
+      </c>
+      <c r="D127" s="44" t="s">
+        <v>856</v>
+      </c>
+      <c r="E127" s="59" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" ht="30">
+      <c r="B128" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C128" s="44"/>
+      <c r="D128" s="44" t="s">
+        <v>854</v>
+      </c>
+      <c r="E128" s="59" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1087" ht="45">
+      <c r="B129" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129" s="44"/>
+      <c r="D129" s="44" t="s">
+        <v>855</v>
+      </c>
+      <c r="E129" s="59" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1087">
+      <c r="B130" s="59"/>
+      <c r="D130" s="44"/>
+      <c r="E130" s="59"/>
+    </row>
+    <row r="131" spans="1:1087">
+      <c r="A131" s="31"/>
+      <c r="B131" s="31"/>
+      <c r="C131" s="31"/>
+      <c r="D131" s="31"/>
+      <c r="E131" s="31"/>
+      <c r="F131" s="31"/>
+      <c r="G131" s="31"/>
+      <c r="H131" s="31"/>
+      <c r="I131" s="31"/>
+      <c r="J131" s="31"/>
+      <c r="K131" s="31"/>
+      <c r="L131" s="31"/>
+      <c r="M131" s="31"/>
+      <c r="N131" s="31"/>
+      <c r="O131" s="31"/>
+      <c r="P131" s="31"/>
+      <c r="Q131" s="31"/>
+      <c r="R131" s="31"/>
+      <c r="S131" s="31"/>
+      <c r="T131" s="31"/>
+      <c r="U131" s="31"/>
+      <c r="V131" s="31"/>
+      <c r="W131" s="31"/>
+      <c r="X131" s="31"/>
+      <c r="Y131" s="31"/>
+      <c r="Z131" s="31"/>
+      <c r="AA131" s="31"/>
+      <c r="AB131" s="31"/>
+      <c r="AC131" s="31"/>
+      <c r="AD131" s="31"/>
+      <c r="AE131" s="31"/>
+      <c r="AF131" s="31"/>
+      <c r="AG131" s="31"/>
+      <c r="AH131" s="31"/>
+      <c r="AI131" s="31"/>
+      <c r="AJ131" s="31"/>
+      <c r="AK131" s="31"/>
+      <c r="AL131" s="31"/>
+      <c r="AM131" s="31"/>
+      <c r="AN131" s="31"/>
+      <c r="AO131" s="31"/>
+      <c r="AP131" s="31"/>
+      <c r="AQ131" s="31"/>
+      <c r="AR131" s="31"/>
+      <c r="AS131" s="31"/>
+      <c r="AT131" s="31"/>
+      <c r="AU131" s="31"/>
+      <c r="AV131" s="31"/>
+      <c r="AW131" s="31"/>
+      <c r="AX131" s="31"/>
+      <c r="AY131" s="31"/>
+      <c r="AZ131" s="31"/>
+      <c r="BA131" s="31"/>
+      <c r="BB131" s="31"/>
+      <c r="BC131" s="31"/>
+      <c r="BD131" s="31"/>
+      <c r="BE131" s="31"/>
+      <c r="BF131" s="31"/>
+      <c r="BG131" s="31"/>
+      <c r="BH131" s="31"/>
+      <c r="BI131" s="31"/>
+      <c r="BJ131" s="31"/>
+      <c r="BK131" s="31"/>
+      <c r="BL131" s="31"/>
+      <c r="BM131" s="31"/>
+      <c r="BN131" s="31"/>
+      <c r="BO131" s="31"/>
+      <c r="BP131" s="31"/>
+      <c r="BQ131" s="31"/>
+      <c r="BR131" s="31"/>
+      <c r="BS131" s="31"/>
+      <c r="BT131" s="31"/>
+      <c r="BU131" s="31"/>
+      <c r="BV131" s="31"/>
+      <c r="BW131" s="31"/>
+      <c r="BX131" s="31"/>
+      <c r="BY131" s="31"/>
+      <c r="BZ131" s="31"/>
+      <c r="CA131" s="31"/>
+      <c r="CB131" s="31"/>
+      <c r="CC131" s="31"/>
+      <c r="CD131" s="31"/>
+      <c r="CE131" s="31"/>
+      <c r="CF131" s="31"/>
+      <c r="CG131" s="31"/>
+      <c r="CH131" s="31"/>
+      <c r="CI131" s="31"/>
+      <c r="CJ131" s="31"/>
+      <c r="CK131" s="31"/>
+      <c r="CL131" s="31"/>
+      <c r="CM131" s="31"/>
+      <c r="CN131" s="31"/>
+      <c r="CO131" s="31"/>
+      <c r="CP131" s="31"/>
+      <c r="CQ131" s="31"/>
+      <c r="CR131" s="31"/>
+      <c r="CS131" s="31"/>
+      <c r="CT131" s="31"/>
+      <c r="CU131" s="31"/>
+      <c r="CV131" s="31"/>
+      <c r="CW131" s="31"/>
+      <c r="CX131" s="31"/>
+      <c r="CY131" s="31"/>
+      <c r="CZ131" s="31"/>
+      <c r="DA131" s="31"/>
+      <c r="DB131" s="31"/>
+      <c r="DC131" s="31"/>
+      <c r="DD131" s="31"/>
+      <c r="DE131" s="31"/>
+      <c r="DF131" s="31"/>
+      <c r="DG131" s="31"/>
+      <c r="DH131" s="31"/>
+      <c r="DI131" s="31"/>
+      <c r="DJ131" s="31"/>
+      <c r="DK131" s="31"/>
+      <c r="DL131" s="31"/>
+      <c r="DM131" s="31"/>
+      <c r="DN131" s="31"/>
+      <c r="DO131" s="31"/>
+      <c r="DP131" s="31"/>
+      <c r="DQ131" s="31"/>
+      <c r="DR131" s="31"/>
+      <c r="DS131" s="31"/>
+      <c r="DT131" s="31"/>
+      <c r="DU131" s="31"/>
+      <c r="DV131" s="31"/>
+      <c r="DW131" s="31"/>
+      <c r="DX131" s="31"/>
+      <c r="DY131" s="31"/>
+      <c r="DZ131" s="31"/>
+      <c r="EA131" s="31"/>
+      <c r="EB131" s="31"/>
+      <c r="EC131" s="31"/>
+      <c r="ED131" s="31"/>
+      <c r="EE131" s="31"/>
+      <c r="EF131" s="31"/>
+      <c r="EG131" s="31"/>
+      <c r="EH131" s="31"/>
+      <c r="EI131" s="31"/>
+      <c r="EJ131" s="31"/>
+      <c r="EK131" s="31"/>
+      <c r="EL131" s="31"/>
+      <c r="EM131" s="31"/>
+      <c r="EN131" s="31"/>
+      <c r="EO131" s="31"/>
+      <c r="EP131" s="31"/>
+      <c r="EQ131" s="31"/>
+      <c r="ER131" s="31"/>
+      <c r="ES131" s="31"/>
+      <c r="ET131" s="31"/>
+      <c r="EU131" s="31"/>
+      <c r="EV131" s="31"/>
+      <c r="EW131" s="31"/>
+      <c r="EX131" s="31"/>
+      <c r="EY131" s="31"/>
+      <c r="EZ131" s="31"/>
+      <c r="FA131" s="31"/>
+      <c r="FB131" s="31"/>
+      <c r="FC131" s="31"/>
+      <c r="FD131" s="31"/>
+      <c r="FE131" s="31"/>
+      <c r="FF131" s="31"/>
+      <c r="FG131" s="31"/>
+      <c r="FH131" s="31"/>
+      <c r="FI131" s="31"/>
+      <c r="FJ131" s="31"/>
+      <c r="FK131" s="31"/>
+      <c r="FL131" s="31"/>
+      <c r="FM131" s="31"/>
+      <c r="FN131" s="31"/>
+      <c r="FO131" s="31"/>
+      <c r="FP131" s="31"/>
+      <c r="FQ131" s="31"/>
+      <c r="FR131" s="31"/>
+      <c r="FS131" s="31"/>
+      <c r="FT131" s="31"/>
+      <c r="FU131" s="31"/>
+      <c r="FV131" s="31"/>
+      <c r="FW131" s="31"/>
+      <c r="FX131" s="31"/>
+      <c r="FY131" s="31"/>
+      <c r="FZ131" s="31"/>
+      <c r="GA131" s="31"/>
+      <c r="GB131" s="31"/>
+      <c r="GC131" s="31"/>
+      <c r="GD131" s="31"/>
+      <c r="GE131" s="31"/>
+      <c r="GF131" s="31"/>
+      <c r="GG131" s="31"/>
+      <c r="GH131" s="31"/>
+      <c r="GI131" s="31"/>
+      <c r="GJ131" s="31"/>
+      <c r="GK131" s="31"/>
+      <c r="GL131" s="31"/>
+      <c r="GM131" s="31"/>
+      <c r="GN131" s="31"/>
+      <c r="GO131" s="31"/>
+      <c r="GP131" s="31"/>
+      <c r="GQ131" s="31"/>
+      <c r="GR131" s="31"/>
+      <c r="GS131" s="31"/>
+      <c r="GT131" s="31"/>
+      <c r="GU131" s="31"/>
+      <c r="GV131" s="31"/>
+      <c r="GW131" s="31"/>
+      <c r="GX131" s="31"/>
+      <c r="GY131" s="31"/>
+      <c r="GZ131" s="31"/>
+      <c r="HA131" s="31"/>
+      <c r="HB131" s="31"/>
+      <c r="HC131" s="31"/>
+      <c r="HD131" s="31"/>
+      <c r="HE131" s="31"/>
+      <c r="HF131" s="31"/>
+      <c r="HG131" s="31"/>
+      <c r="HH131" s="31"/>
+      <c r="HI131" s="31"/>
+      <c r="HJ131" s="31"/>
+      <c r="HK131" s="31"/>
+      <c r="HL131" s="31"/>
+      <c r="HM131" s="31"/>
+      <c r="HN131" s="31"/>
+      <c r="HO131" s="31"/>
+      <c r="HP131" s="31"/>
+      <c r="HQ131" s="31"/>
+      <c r="HR131" s="31"/>
+      <c r="HS131" s="31"/>
+      <c r="HT131" s="31"/>
+      <c r="HU131" s="31"/>
+      <c r="HV131" s="31"/>
+      <c r="HW131" s="31"/>
+      <c r="HX131" s="31"/>
+      <c r="HY131" s="31"/>
+      <c r="HZ131" s="31"/>
+      <c r="IA131" s="31"/>
+      <c r="IB131" s="31"/>
+      <c r="IC131" s="31"/>
+      <c r="ID131" s="31"/>
+      <c r="IE131" s="31"/>
+      <c r="IF131" s="31"/>
+      <c r="IG131" s="31"/>
+      <c r="IH131" s="31"/>
+      <c r="II131" s="31"/>
+      <c r="IJ131" s="31"/>
+      <c r="IK131" s="31"/>
+      <c r="IL131" s="31"/>
+      <c r="IM131" s="31"/>
+      <c r="IN131" s="31"/>
+      <c r="IO131" s="31"/>
+      <c r="IP131" s="31"/>
+      <c r="IQ131" s="31"/>
+      <c r="IR131" s="31"/>
+      <c r="IS131" s="31"/>
+      <c r="IT131" s="31"/>
+      <c r="IU131" s="31"/>
+      <c r="IV131" s="31"/>
+      <c r="IW131" s="31"/>
+      <c r="IX131" s="31"/>
+      <c r="IY131" s="31"/>
+      <c r="IZ131" s="31"/>
+      <c r="JA131" s="31"/>
+      <c r="JB131" s="31"/>
+      <c r="JC131" s="31"/>
+      <c r="JD131" s="31"/>
+      <c r="JE131" s="31"/>
+      <c r="JF131" s="31"/>
+      <c r="JG131" s="31"/>
+      <c r="JH131" s="31"/>
+      <c r="JI131" s="31"/>
+      <c r="JJ131" s="31"/>
+      <c r="JK131" s="31"/>
+      <c r="JL131" s="31"/>
+      <c r="JM131" s="31"/>
+      <c r="JN131" s="31"/>
+      <c r="JO131" s="31"/>
+      <c r="JP131" s="31"/>
+      <c r="JQ131" s="31"/>
+      <c r="JR131" s="31"/>
+      <c r="JS131" s="31"/>
+      <c r="JT131" s="31"/>
+      <c r="JU131" s="31"/>
+      <c r="JV131" s="31"/>
+      <c r="JW131" s="31"/>
+      <c r="JX131" s="31"/>
+      <c r="JY131" s="31"/>
+      <c r="JZ131" s="31"/>
+      <c r="KA131" s="31"/>
+      <c r="KB131" s="31"/>
+      <c r="KC131" s="31"/>
+      <c r="KD131" s="31"/>
+      <c r="KE131" s="31"/>
+      <c r="KF131" s="31"/>
+      <c r="KG131" s="31"/>
+      <c r="KH131" s="31"/>
+      <c r="KI131" s="31"/>
+      <c r="KJ131" s="31"/>
+      <c r="KK131" s="31"/>
+      <c r="KL131" s="31"/>
+      <c r="KM131" s="31"/>
+      <c r="KN131" s="31"/>
+      <c r="KO131" s="31"/>
+      <c r="KP131" s="31"/>
+      <c r="KQ131" s="31"/>
+      <c r="KR131" s="31"/>
+      <c r="KS131" s="31"/>
+      <c r="KT131" s="31"/>
+      <c r="KU131" s="31"/>
+      <c r="KV131" s="31"/>
+      <c r="KW131" s="31"/>
+      <c r="KX131" s="31"/>
+      <c r="KY131" s="31"/>
+      <c r="KZ131" s="31"/>
+      <c r="LA131" s="31"/>
+      <c r="LB131" s="31"/>
+      <c r="LC131" s="31"/>
+      <c r="LD131" s="31"/>
+      <c r="LE131" s="31"/>
+      <c r="LF131" s="31"/>
+      <c r="LG131" s="31"/>
+      <c r="LH131" s="31"/>
+      <c r="LI131" s="31"/>
+      <c r="LJ131" s="31"/>
+      <c r="LK131" s="31"/>
+      <c r="LL131" s="31"/>
+      <c r="LM131" s="31"/>
+      <c r="LN131" s="31"/>
+      <c r="LO131" s="31"/>
+      <c r="LP131" s="31"/>
+      <c r="LQ131" s="31"/>
+      <c r="LR131" s="31"/>
+      <c r="LS131" s="31"/>
+      <c r="LT131" s="31"/>
+      <c r="LU131" s="31"/>
+      <c r="LV131" s="31"/>
+      <c r="LW131" s="31"/>
+      <c r="LX131" s="31"/>
+      <c r="LY131" s="31"/>
+      <c r="LZ131" s="31"/>
+      <c r="MA131" s="31"/>
+      <c r="MB131" s="31"/>
+      <c r="MC131" s="31"/>
+      <c r="MD131" s="31"/>
+      <c r="ME131" s="31"/>
+      <c r="MF131" s="31"/>
+      <c r="MG131" s="31"/>
+      <c r="MH131" s="31"/>
+      <c r="MI131" s="31"/>
+      <c r="MJ131" s="31"/>
+      <c r="MK131" s="31"/>
+      <c r="ML131" s="31"/>
+      <c r="MM131" s="31"/>
+      <c r="MN131" s="31"/>
+      <c r="MO131" s="31"/>
+      <c r="MP131" s="31"/>
+      <c r="MQ131" s="31"/>
+      <c r="MR131" s="31"/>
+      <c r="MS131" s="31"/>
+      <c r="MT131" s="31"/>
+      <c r="MU131" s="31"/>
+      <c r="MV131" s="31"/>
+      <c r="MW131" s="31"/>
+      <c r="MX131" s="31"/>
+      <c r="MY131" s="31"/>
+      <c r="MZ131" s="31"/>
+      <c r="NA131" s="31"/>
+      <c r="NB131" s="31"/>
+      <c r="NC131" s="31"/>
+      <c r="ND131" s="31"/>
+      <c r="NE131" s="31"/>
+      <c r="NF131" s="31"/>
+      <c r="NG131" s="31"/>
+      <c r="NH131" s="31"/>
+      <c r="NI131" s="31"/>
+      <c r="NJ131" s="31"/>
+      <c r="NK131" s="31"/>
+      <c r="NL131" s="31"/>
+      <c r="NM131" s="31"/>
+      <c r="NN131" s="31"/>
+      <c r="NO131" s="31"/>
+      <c r="NP131" s="31"/>
+      <c r="NQ131" s="31"/>
+      <c r="NR131" s="31"/>
+      <c r="NS131" s="31"/>
+      <c r="NT131" s="31"/>
+      <c r="NU131" s="31"/>
+      <c r="NV131" s="31"/>
+      <c r="NW131" s="31"/>
+      <c r="NX131" s="31"/>
+      <c r="NY131" s="31"/>
+      <c r="NZ131" s="31"/>
+      <c r="OA131" s="31"/>
+      <c r="OB131" s="31"/>
+      <c r="OC131" s="31"/>
+      <c r="OD131" s="31"/>
+      <c r="OE131" s="31"/>
+      <c r="OF131" s="31"/>
+      <c r="OG131" s="31"/>
+      <c r="OH131" s="31"/>
+      <c r="OI131" s="31"/>
+      <c r="OJ131" s="31"/>
+      <c r="OK131" s="31"/>
+      <c r="OL131" s="31"/>
+      <c r="OM131" s="31"/>
+      <c r="ON131" s="31"/>
+      <c r="OO131" s="31"/>
+      <c r="OP131" s="31"/>
+      <c r="OQ131" s="31"/>
+      <c r="OR131" s="31"/>
+      <c r="OS131" s="31"/>
+      <c r="OT131" s="31"/>
+      <c r="OU131" s="31"/>
+      <c r="OV131" s="31"/>
+      <c r="OW131" s="31"/>
+      <c r="OX131" s="31"/>
+      <c r="OY131" s="31"/>
+      <c r="OZ131" s="31"/>
+      <c r="PA131" s="31"/>
+      <c r="PB131" s="31"/>
+      <c r="PC131" s="31"/>
+      <c r="PD131" s="31"/>
+      <c r="PE131" s="31"/>
+      <c r="PF131" s="31"/>
+      <c r="PG131" s="31"/>
+      <c r="PH131" s="31"/>
+      <c r="PI131" s="31"/>
+      <c r="PJ131" s="31"/>
+      <c r="PK131" s="31"/>
+      <c r="PL131" s="31"/>
+      <c r="PM131" s="31"/>
+      <c r="PN131" s="31"/>
+      <c r="PO131" s="31"/>
+      <c r="PP131" s="31"/>
+      <c r="PQ131" s="31"/>
+      <c r="PR131" s="31"/>
+      <c r="PS131" s="31"/>
+      <c r="PT131" s="31"/>
+      <c r="PU131" s="31"/>
+      <c r="PV131" s="31"/>
+      <c r="PW131" s="31"/>
+      <c r="PX131" s="31"/>
+      <c r="PY131" s="31"/>
+      <c r="PZ131" s="31"/>
+      <c r="QA131" s="31"/>
+      <c r="QB131" s="31"/>
+      <c r="QC131" s="31"/>
+      <c r="QD131" s="31"/>
+      <c r="QE131" s="31"/>
+      <c r="QF131" s="31"/>
+      <c r="QG131" s="31"/>
+      <c r="QH131" s="31"/>
+      <c r="QI131" s="31"/>
+      <c r="QJ131" s="31"/>
+      <c r="QK131" s="31"/>
+      <c r="QL131" s="31"/>
+      <c r="QM131" s="31"/>
+      <c r="QN131" s="31"/>
+      <c r="QO131" s="31"/>
+      <c r="QP131" s="31"/>
+      <c r="QQ131" s="31"/>
+      <c r="QR131" s="31"/>
+      <c r="QS131" s="31"/>
+      <c r="QT131" s="31"/>
+      <c r="QU131" s="31"/>
+      <c r="QV131" s="31"/>
+      <c r="QW131" s="31"/>
+      <c r="QX131" s="31"/>
+      <c r="QY131" s="31"/>
+      <c r="QZ131" s="31"/>
+      <c r="RA131" s="31"/>
+      <c r="RB131" s="31"/>
+      <c r="RC131" s="31"/>
+      <c r="RD131" s="31"/>
+      <c r="RE131" s="31"/>
+      <c r="RF131" s="31"/>
+      <c r="RG131" s="31"/>
+      <c r="RH131" s="31"/>
+      <c r="RI131" s="31"/>
+      <c r="RJ131" s="31"/>
+      <c r="RK131" s="31"/>
+      <c r="RL131" s="31"/>
+      <c r="RM131" s="31"/>
+      <c r="RN131" s="31"/>
+      <c r="RO131" s="31"/>
+      <c r="RP131" s="31"/>
+      <c r="RQ131" s="31"/>
+      <c r="RR131" s="31"/>
+      <c r="RS131" s="31"/>
+      <c r="RT131" s="31"/>
+      <c r="RU131" s="31"/>
+      <c r="RV131" s="31"/>
+      <c r="RW131" s="31"/>
+      <c r="RX131" s="31"/>
+      <c r="RY131" s="31"/>
+      <c r="RZ131" s="31"/>
+      <c r="SA131" s="31"/>
+      <c r="SB131" s="31"/>
+      <c r="SC131" s="31"/>
+      <c r="SD131" s="31"/>
+      <c r="SE131" s="31"/>
+      <c r="SF131" s="31"/>
+      <c r="SG131" s="31"/>
+      <c r="SH131" s="31"/>
+      <c r="SI131" s="31"/>
+      <c r="SJ131" s="31"/>
+      <c r="SK131" s="31"/>
+      <c r="SL131" s="31"/>
+      <c r="SM131" s="31"/>
+      <c r="SN131" s="31"/>
+      <c r="SO131" s="31"/>
+      <c r="SP131" s="31"/>
+      <c r="SQ131" s="31"/>
+      <c r="SR131" s="31"/>
+      <c r="SS131" s="31"/>
+      <c r="ST131" s="31"/>
+      <c r="SU131" s="31"/>
+      <c r="SV131" s="31"/>
+      <c r="SW131" s="31"/>
+      <c r="SX131" s="31"/>
+      <c r="SY131" s="31"/>
+      <c r="SZ131" s="31"/>
+      <c r="TA131" s="31"/>
+      <c r="TB131" s="31"/>
+      <c r="TC131" s="31"/>
+      <c r="TD131" s="31"/>
+      <c r="TE131" s="31"/>
+      <c r="TF131" s="31"/>
+      <c r="TG131" s="31"/>
+      <c r="TH131" s="31"/>
+      <c r="TI131" s="31"/>
+      <c r="TJ131" s="31"/>
+      <c r="TK131" s="31"/>
+      <c r="TL131" s="31"/>
+      <c r="TM131" s="31"/>
+      <c r="TN131" s="31"/>
+      <c r="TO131" s="31"/>
+      <c r="TP131" s="31"/>
+      <c r="TQ131" s="31"/>
+      <c r="TR131" s="31"/>
+      <c r="TS131" s="31"/>
+      <c r="TT131" s="31"/>
+      <c r="TU131" s="31"/>
+      <c r="TV131" s="31"/>
+      <c r="TW131" s="31"/>
+      <c r="TX131" s="31"/>
+      <c r="TY131" s="31"/>
+      <c r="TZ131" s="31"/>
+      <c r="UA131" s="31"/>
+      <c r="UB131" s="31"/>
+      <c r="UC131" s="31"/>
+      <c r="UD131" s="31"/>
+      <c r="UE131" s="31"/>
+      <c r="UF131" s="31"/>
+      <c r="UG131" s="31"/>
+      <c r="UH131" s="31"/>
+      <c r="UI131" s="31"/>
+      <c r="UJ131" s="31"/>
+      <c r="UK131" s="31"/>
+      <c r="UL131" s="31"/>
+      <c r="UM131" s="31"/>
+      <c r="UN131" s="31"/>
+      <c r="UO131" s="31"/>
+      <c r="UP131" s="31"/>
+      <c r="UQ131" s="31"/>
+      <c r="UR131" s="31"/>
+      <c r="US131" s="31"/>
+      <c r="UT131" s="31"/>
+      <c r="UU131" s="31"/>
+      <c r="UV131" s="31"/>
+      <c r="UW131" s="31"/>
+      <c r="UX131" s="31"/>
+      <c r="UY131" s="31"/>
+      <c r="UZ131" s="31"/>
+      <c r="VA131" s="31"/>
+      <c r="VB131" s="31"/>
+      <c r="VC131" s="31"/>
+      <c r="VD131" s="31"/>
+      <c r="VE131" s="31"/>
+      <c r="VF131" s="31"/>
+      <c r="VG131" s="31"/>
+      <c r="VH131" s="31"/>
+      <c r="VI131" s="31"/>
+      <c r="VJ131" s="31"/>
+      <c r="VK131" s="31"/>
+      <c r="VL131" s="31"/>
+      <c r="VM131" s="31"/>
+      <c r="VN131" s="31"/>
+      <c r="VO131" s="31"/>
+      <c r="VP131" s="31"/>
+      <c r="VQ131" s="31"/>
+      <c r="VR131" s="31"/>
+      <c r="VS131" s="31"/>
+      <c r="VT131" s="31"/>
+      <c r="VU131" s="31"/>
+      <c r="VV131" s="31"/>
+      <c r="VW131" s="31"/>
+      <c r="VX131" s="31"/>
+      <c r="VY131" s="31"/>
+      <c r="VZ131" s="31"/>
+      <c r="WA131" s="31"/>
+      <c r="WB131" s="31"/>
+      <c r="WC131" s="31"/>
+      <c r="WD131" s="31"/>
+      <c r="WE131" s="31"/>
+      <c r="WF131" s="31"/>
+      <c r="WG131" s="31"/>
+      <c r="WH131" s="31"/>
+      <c r="WI131" s="31"/>
+      <c r="WJ131" s="31"/>
+      <c r="WK131" s="31"/>
+      <c r="WL131" s="31"/>
+      <c r="WM131" s="31"/>
+      <c r="WN131" s="31"/>
+      <c r="WO131" s="31"/>
+      <c r="WP131" s="31"/>
+      <c r="WQ131" s="31"/>
+      <c r="WR131" s="31"/>
+      <c r="WS131" s="31"/>
+      <c r="WT131" s="31"/>
+      <c r="WU131" s="31"/>
+      <c r="WV131" s="31"/>
+      <c r="WW131" s="31"/>
+      <c r="WX131" s="31"/>
+      <c r="WY131" s="31"/>
+      <c r="WZ131" s="31"/>
+      <c r="XA131" s="31"/>
+      <c r="XB131" s="31"/>
+      <c r="XC131" s="31"/>
+      <c r="XD131" s="31"/>
+      <c r="XE131" s="31"/>
+      <c r="XF131" s="31"/>
+      <c r="XG131" s="31"/>
+      <c r="XH131" s="31"/>
+      <c r="XI131" s="31"/>
+      <c r="XJ131" s="31"/>
+      <c r="XK131" s="31"/>
+      <c r="XL131" s="31"/>
+      <c r="XM131" s="31"/>
+      <c r="XN131" s="31"/>
+      <c r="XO131" s="31"/>
+      <c r="XP131" s="31"/>
+      <c r="XQ131" s="31"/>
+      <c r="XR131" s="31"/>
+      <c r="XS131" s="31"/>
+      <c r="XT131" s="31"/>
+      <c r="XU131" s="31"/>
+      <c r="XV131" s="31"/>
+      <c r="XW131" s="31"/>
+      <c r="XX131" s="31"/>
+      <c r="XY131" s="31"/>
+      <c r="XZ131" s="31"/>
+      <c r="YA131" s="31"/>
+      <c r="YB131" s="31"/>
+      <c r="YC131" s="31"/>
+      <c r="YD131" s="31"/>
+      <c r="YE131" s="31"/>
+      <c r="YF131" s="31"/>
+      <c r="YG131" s="31"/>
+      <c r="YH131" s="31"/>
+      <c r="YI131" s="31"/>
+      <c r="YJ131" s="31"/>
+      <c r="YK131" s="31"/>
+      <c r="YL131" s="31"/>
+      <c r="YM131" s="31"/>
+      <c r="YN131" s="31"/>
+      <c r="YO131" s="31"/>
+      <c r="YP131" s="31"/>
+      <c r="YQ131" s="31"/>
+      <c r="YR131" s="31"/>
+      <c r="YS131" s="31"/>
+      <c r="YT131" s="31"/>
+      <c r="YU131" s="31"/>
+      <c r="YV131" s="31"/>
+      <c r="YW131" s="31"/>
+      <c r="YX131" s="31"/>
+      <c r="YY131" s="31"/>
+      <c r="YZ131" s="31"/>
+      <c r="ZA131" s="31"/>
+      <c r="ZB131" s="31"/>
+      <c r="ZC131" s="31"/>
+      <c r="ZD131" s="31"/>
+      <c r="ZE131" s="31"/>
+      <c r="ZF131" s="31"/>
+      <c r="ZG131" s="31"/>
+      <c r="ZH131" s="31"/>
+      <c r="ZI131" s="31"/>
+      <c r="ZJ131" s="31"/>
+      <c r="ZK131" s="31"/>
+      <c r="ZL131" s="31"/>
+      <c r="ZM131" s="31"/>
+      <c r="ZN131" s="31"/>
+      <c r="ZO131" s="31"/>
+      <c r="ZP131" s="31"/>
+      <c r="ZQ131" s="31"/>
+      <c r="ZR131" s="31"/>
+      <c r="ZS131" s="31"/>
+      <c r="ZT131" s="31"/>
+      <c r="ZU131" s="31"/>
+      <c r="ZV131" s="31"/>
+      <c r="ZW131" s="31"/>
+      <c r="ZX131" s="31"/>
+      <c r="ZY131" s="31"/>
+      <c r="ZZ131" s="31"/>
+      <c r="AAA131" s="31"/>
+      <c r="AAB131" s="31"/>
+      <c r="AAC131" s="31"/>
+      <c r="AAD131" s="31"/>
+      <c r="AAE131" s="31"/>
+      <c r="AAF131" s="31"/>
+      <c r="AAG131" s="31"/>
+      <c r="AAH131" s="31"/>
+      <c r="AAI131" s="31"/>
+      <c r="AAJ131" s="31"/>
+      <c r="AAK131" s="31"/>
+      <c r="AAL131" s="31"/>
+      <c r="AAM131" s="31"/>
+      <c r="AAN131" s="31"/>
+      <c r="AAO131" s="31"/>
+      <c r="AAP131" s="31"/>
+      <c r="AAQ131" s="31"/>
+      <c r="AAR131" s="31"/>
+      <c r="AAS131" s="31"/>
+      <c r="AAT131" s="31"/>
+      <c r="AAU131" s="31"/>
+      <c r="AAV131" s="31"/>
+      <c r="AAW131" s="31"/>
+      <c r="AAX131" s="31"/>
+      <c r="AAY131" s="31"/>
+      <c r="AAZ131" s="31"/>
+      <c r="ABA131" s="31"/>
+      <c r="ABB131" s="31"/>
+      <c r="ABC131" s="31"/>
+      <c r="ABD131" s="31"/>
+      <c r="ABE131" s="31"/>
+      <c r="ABF131" s="31"/>
+      <c r="ABG131" s="31"/>
+      <c r="ABH131" s="31"/>
+      <c r="ABI131" s="31"/>
+      <c r="ABJ131" s="31"/>
+      <c r="ABK131" s="31"/>
+      <c r="ABL131" s="31"/>
+      <c r="ABM131" s="31"/>
+      <c r="ABN131" s="31"/>
+      <c r="ABO131" s="31"/>
+      <c r="ABP131" s="31"/>
+      <c r="ABQ131" s="31"/>
+      <c r="ABR131" s="31"/>
+      <c r="ABS131" s="31"/>
+      <c r="ABT131" s="31"/>
+      <c r="ABU131" s="31"/>
+      <c r="ABV131" s="31"/>
+      <c r="ABW131" s="31"/>
+      <c r="ABX131" s="31"/>
+      <c r="ABY131" s="31"/>
+      <c r="ABZ131" s="31"/>
+      <c r="ACA131" s="31"/>
+      <c r="ACB131" s="31"/>
+      <c r="ACC131" s="31"/>
+      <c r="ACD131" s="31"/>
+      <c r="ACE131" s="31"/>
+      <c r="ACF131" s="31"/>
+      <c r="ACG131" s="31"/>
+      <c r="ACH131" s="31"/>
+      <c r="ACI131" s="31"/>
+      <c r="ACJ131" s="31"/>
+      <c r="ACK131" s="31"/>
+      <c r="ACL131" s="31"/>
+      <c r="ACM131" s="31"/>
+      <c r="ACN131" s="31"/>
+      <c r="ACO131" s="31"/>
+      <c r="ACP131" s="31"/>
+      <c r="ACQ131" s="31"/>
+      <c r="ACR131" s="31"/>
+      <c r="ACS131" s="31"/>
+      <c r="ACT131" s="31"/>
+      <c r="ACU131" s="31"/>
+      <c r="ACV131" s="31"/>
+      <c r="ACW131" s="31"/>
+      <c r="ACX131" s="31"/>
+      <c r="ACY131" s="31"/>
+      <c r="ACZ131" s="31"/>
+      <c r="ADA131" s="31"/>
+      <c r="ADB131" s="31"/>
+      <c r="ADC131" s="31"/>
+      <c r="ADD131" s="31"/>
+      <c r="ADE131" s="31"/>
+      <c r="ADF131" s="31"/>
+      <c r="ADG131" s="31"/>
+      <c r="ADH131" s="31"/>
+      <c r="ADI131" s="31"/>
+      <c r="ADJ131" s="31"/>
+      <c r="ADK131" s="31"/>
+      <c r="ADL131" s="31"/>
+      <c r="ADM131" s="31"/>
+      <c r="ADN131" s="31"/>
+      <c r="ADO131" s="31"/>
+      <c r="ADP131" s="31"/>
+      <c r="ADQ131" s="31"/>
+      <c r="ADR131" s="31"/>
+      <c r="ADS131" s="31"/>
+      <c r="ADT131" s="31"/>
+      <c r="ADU131" s="31"/>
+      <c r="ADV131" s="31"/>
+      <c r="ADW131" s="31"/>
+      <c r="ADX131" s="31"/>
+      <c r="ADY131" s="31"/>
+      <c r="ADZ131" s="31"/>
+      <c r="AEA131" s="31"/>
+      <c r="AEB131" s="31"/>
+      <c r="AEC131" s="31"/>
+      <c r="AED131" s="31"/>
+      <c r="AEE131" s="31"/>
+      <c r="AEF131" s="31"/>
+      <c r="AEG131" s="31"/>
+      <c r="AEH131" s="31"/>
+      <c r="AEI131" s="31"/>
+      <c r="AEJ131" s="31"/>
+      <c r="AEK131" s="31"/>
+      <c r="AEL131" s="31"/>
+      <c r="AEM131" s="31"/>
+      <c r="AEN131" s="31"/>
+      <c r="AEO131" s="31"/>
+      <c r="AEP131" s="31"/>
+      <c r="AEQ131" s="31"/>
+      <c r="AER131" s="31"/>
+      <c r="AES131" s="31"/>
+      <c r="AET131" s="31"/>
+      <c r="AEU131" s="31"/>
+      <c r="AEV131" s="31"/>
+      <c r="AEW131" s="31"/>
+      <c r="AEX131" s="31"/>
+      <c r="AEY131" s="31"/>
+      <c r="AEZ131" s="31"/>
+      <c r="AFA131" s="31"/>
+      <c r="AFB131" s="31"/>
+      <c r="AFC131" s="31"/>
+      <c r="AFD131" s="31"/>
+      <c r="AFE131" s="31"/>
+      <c r="AFF131" s="31"/>
+      <c r="AFG131" s="31"/>
+      <c r="AFH131" s="31"/>
+      <c r="AFI131" s="31"/>
+      <c r="AFJ131" s="31"/>
+      <c r="AFK131" s="31"/>
+      <c r="AFL131" s="31"/>
+      <c r="AFM131" s="31"/>
+      <c r="AFN131" s="31"/>
+      <c r="AFO131" s="31"/>
+      <c r="AFP131" s="31"/>
+      <c r="AFQ131" s="31"/>
+      <c r="AFR131" s="31"/>
+      <c r="AFS131" s="31"/>
+      <c r="AFT131" s="31"/>
+      <c r="AFU131" s="31"/>
+      <c r="AFV131" s="31"/>
+      <c r="AFW131" s="31"/>
+      <c r="AFX131" s="31"/>
+      <c r="AFY131" s="31"/>
+      <c r="AFZ131" s="31"/>
+      <c r="AGA131" s="31"/>
+      <c r="AGB131" s="31"/>
+      <c r="AGC131" s="31"/>
+      <c r="AGD131" s="31"/>
+      <c r="AGE131" s="31"/>
+      <c r="AGF131" s="31"/>
+      <c r="AGG131" s="31"/>
+      <c r="AGH131" s="31"/>
+      <c r="AGI131" s="31"/>
+      <c r="AGJ131" s="31"/>
+      <c r="AGK131" s="31"/>
+      <c r="AGL131" s="31"/>
+      <c r="AGM131" s="31"/>
+      <c r="AGN131" s="31"/>
+      <c r="AGO131" s="31"/>
+      <c r="AGP131" s="31"/>
+      <c r="AGQ131" s="31"/>
+      <c r="AGR131" s="31"/>
+      <c r="AGS131" s="31"/>
+      <c r="AGT131" s="31"/>
+      <c r="AGU131" s="31"/>
+      <c r="AGV131" s="31"/>
+      <c r="AGW131" s="31"/>
+      <c r="AGX131" s="31"/>
+      <c r="AGY131" s="31"/>
+      <c r="AGZ131" s="31"/>
+      <c r="AHA131" s="31"/>
+      <c r="AHB131" s="31"/>
+      <c r="AHC131" s="31"/>
+      <c r="AHD131" s="31"/>
+      <c r="AHE131" s="31"/>
+      <c r="AHF131" s="31"/>
+      <c r="AHG131" s="31"/>
+      <c r="AHH131" s="31"/>
+      <c r="AHI131" s="31"/>
+      <c r="AHJ131" s="31"/>
+      <c r="AHK131" s="31"/>
+      <c r="AHL131" s="31"/>
+      <c r="AHM131" s="31"/>
+      <c r="AHN131" s="31"/>
+      <c r="AHO131" s="31"/>
+      <c r="AHP131" s="31"/>
+      <c r="AHQ131" s="31"/>
+      <c r="AHR131" s="31"/>
+      <c r="AHS131" s="31"/>
+      <c r="AHT131" s="31"/>
+      <c r="AHU131" s="31"/>
+      <c r="AHV131" s="31"/>
+      <c r="AHW131" s="31"/>
+      <c r="AHX131" s="31"/>
+      <c r="AHY131" s="31"/>
+      <c r="AHZ131" s="31"/>
+      <c r="AIA131" s="31"/>
+      <c r="AIB131" s="31"/>
+      <c r="AIC131" s="31"/>
+      <c r="AID131" s="31"/>
+      <c r="AIE131" s="31"/>
+      <c r="AIF131" s="31"/>
+      <c r="AIG131" s="31"/>
+      <c r="AIH131" s="31"/>
+      <c r="AII131" s="31"/>
+      <c r="AIJ131" s="31"/>
+      <c r="AIK131" s="31"/>
+      <c r="AIL131" s="31"/>
+      <c r="AIM131" s="31"/>
+      <c r="AIN131" s="31"/>
+      <c r="AIO131" s="31"/>
+      <c r="AIP131" s="31"/>
+      <c r="AIQ131" s="31"/>
+      <c r="AIR131" s="31"/>
+      <c r="AIS131" s="31"/>
+      <c r="AIT131" s="31"/>
+      <c r="AIU131" s="31"/>
+      <c r="AIV131" s="31"/>
+      <c r="AIW131" s="31"/>
+      <c r="AIX131" s="31"/>
+      <c r="AIY131" s="31"/>
+      <c r="AIZ131" s="31"/>
+      <c r="AJA131" s="31"/>
+      <c r="AJB131" s="31"/>
+      <c r="AJC131" s="31"/>
+      <c r="AJD131" s="31"/>
+      <c r="AJE131" s="31"/>
+      <c r="AJF131" s="31"/>
+      <c r="AJG131" s="31"/>
+      <c r="AJH131" s="31"/>
+      <c r="AJI131" s="31"/>
+      <c r="AJJ131" s="31"/>
+      <c r="AJK131" s="31"/>
+      <c r="AJL131" s="31"/>
+      <c r="AJM131" s="31"/>
+      <c r="AJN131" s="31"/>
+      <c r="AJO131" s="31"/>
+      <c r="AJP131" s="31"/>
+      <c r="AJQ131" s="31"/>
+      <c r="AJR131" s="31"/>
+      <c r="AJS131" s="31"/>
+      <c r="AJT131" s="31"/>
+      <c r="AJU131" s="31"/>
+      <c r="AJV131" s="31"/>
+      <c r="AJW131" s="31"/>
+      <c r="AJX131" s="31"/>
+      <c r="AJY131" s="31"/>
+      <c r="AJZ131" s="31"/>
+      <c r="AKA131" s="31"/>
+      <c r="AKB131" s="31"/>
+      <c r="AKC131" s="31"/>
+      <c r="AKD131" s="31"/>
+      <c r="AKE131" s="31"/>
+      <c r="AKF131" s="31"/>
+      <c r="AKG131" s="31"/>
+      <c r="AKH131" s="31"/>
+      <c r="AKI131" s="31"/>
+      <c r="AKJ131" s="31"/>
+      <c r="AKK131" s="31"/>
+      <c r="AKL131" s="31"/>
+      <c r="AKM131" s="31"/>
+      <c r="AKN131" s="31"/>
+      <c r="AKO131" s="31"/>
+      <c r="AKP131" s="31"/>
+      <c r="AKQ131" s="31"/>
+      <c r="AKR131" s="31"/>
+      <c r="AKS131" s="31"/>
+      <c r="AKT131" s="31"/>
+      <c r="AKU131" s="31"/>
+      <c r="AKV131" s="31"/>
+      <c r="AKW131" s="31"/>
+      <c r="AKX131" s="31"/>
+      <c r="AKY131" s="31"/>
+      <c r="AKZ131" s="31"/>
+      <c r="ALA131" s="31"/>
+      <c r="ALB131" s="31"/>
+      <c r="ALC131" s="31"/>
+      <c r="ALD131" s="31"/>
+      <c r="ALE131" s="31"/>
+      <c r="ALF131" s="31"/>
+      <c r="ALG131" s="31"/>
+      <c r="ALH131" s="31"/>
+      <c r="ALI131" s="31"/>
+      <c r="ALJ131" s="31"/>
+      <c r="ALK131" s="31"/>
+      <c r="ALL131" s="31"/>
+      <c r="ALM131" s="31"/>
+      <c r="ALN131" s="31"/>
+      <c r="ALO131" s="31"/>
+      <c r="ALP131" s="31"/>
+      <c r="ALQ131" s="31"/>
+      <c r="ALR131" s="31"/>
+      <c r="ALS131" s="31"/>
+      <c r="ALT131" s="31"/>
+      <c r="ALU131" s="31"/>
+      <c r="ALV131" s="31"/>
+      <c r="ALW131" s="31"/>
+      <c r="ALX131" s="31"/>
+      <c r="ALY131" s="31"/>
+      <c r="ALZ131" s="31"/>
+      <c r="AMA131" s="31"/>
+      <c r="AMB131" s="31"/>
+      <c r="AMC131" s="31"/>
+      <c r="AMD131" s="31"/>
+      <c r="AME131" s="31"/>
+      <c r="AMF131" s="31"/>
+      <c r="AMG131" s="31"/>
+      <c r="AMH131" s="31"/>
+      <c r="AMI131" s="31"/>
+      <c r="AMJ131" s="31"/>
+      <c r="AMK131" s="31"/>
+      <c r="AML131" s="31"/>
+      <c r="AMM131" s="31"/>
+      <c r="AMN131" s="31"/>
+      <c r="AMO131" s="31"/>
+      <c r="AMP131" s="31"/>
+      <c r="AMQ131" s="31"/>
+      <c r="AMR131" s="31"/>
+      <c r="AMS131" s="31"/>
+      <c r="AMT131" s="31"/>
+      <c r="AMU131" s="31"/>
+      <c r="AMV131" s="31"/>
+      <c r="AMW131" s="31"/>
+      <c r="AMX131" s="31"/>
+      <c r="AMY131" s="31"/>
+      <c r="AMZ131" s="31"/>
+      <c r="ANA131" s="31"/>
+      <c r="ANB131" s="31"/>
+      <c r="ANC131" s="31"/>
+      <c r="AND131" s="31"/>
+      <c r="ANE131" s="31"/>
+      <c r="ANF131" s="31"/>
+      <c r="ANG131" s="31"/>
+      <c r="ANH131" s="31"/>
+      <c r="ANI131" s="31"/>
+      <c r="ANJ131" s="31"/>
+      <c r="ANK131" s="31"/>
+      <c r="ANL131" s="31"/>
+      <c r="ANM131" s="31"/>
+      <c r="ANN131" s="31"/>
+      <c r="ANO131" s="31"/>
+      <c r="ANP131" s="31"/>
+      <c r="ANQ131" s="31"/>
+      <c r="ANR131" s="31"/>
+      <c r="ANS131" s="31"/>
+      <c r="ANT131" s="31"/>
+      <c r="ANU131" s="31"/>
+      <c r="ANV131" s="31"/>
+      <c r="ANW131" s="31"/>
+      <c r="ANX131" s="31"/>
+      <c r="ANY131" s="31"/>
+      <c r="ANZ131" s="31"/>
+      <c r="AOA131" s="31"/>
+      <c r="AOB131" s="31"/>
+      <c r="AOC131" s="31"/>
+      <c r="AOD131" s="31"/>
+      <c r="AOE131" s="31"/>
+      <c r="AOF131" s="31"/>
+      <c r="AOG131" s="31"/>
+      <c r="AOH131" s="31"/>
+      <c r="AOI131" s="31"/>
+      <c r="AOJ131" s="31"/>
+      <c r="AOK131" s="31"/>
+      <c r="AOL131" s="31"/>
+      <c r="AOM131" s="31"/>
+      <c r="AON131" s="31"/>
+      <c r="AOO131" s="31"/>
+      <c r="AOP131" s="31"/>
+      <c r="AOQ131" s="31"/>
+      <c r="AOR131" s="31"/>
+      <c r="AOS131" s="31"/>
+      <c r="AOT131" s="31"/>
+      <c r="AOU131" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B103:C103"/>
     <mergeCell ref="B124:C124"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A3:C3"/>
@@ -86918,9 +86979,6 @@
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="B119:C119"/>
     <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B103:C103"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70833333333333304" right="1.1000000000000001" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>